<commit_message>
version 2.0 of the model and visualization software
</commit_message>
<xml_diff>
--- a/Sean/Trials/Hyperparameters.xlsx
+++ b/Sean/Trials/Hyperparameters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="42">
   <si>
     <t>Trial #</t>
   </si>
@@ -109,10 +109,37 @@
     <t>[0.11485175043344498, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827, 0.28534170985221863, 0.3073540925979614, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827, 0.3081763982772827]</t>
   </si>
   <si>
+    <t>[0.2407248467206955, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.2735336124897003, 0.27448737621307373, 0.29566046595573425, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30548402667045593, 0.30815449357032776, 0.3078683912754059, 0.3083452582359314, 0.3058655261993408, 0.3065331280231476, 0.3067238926887512, 0.30805912613868713, 0.30739152431488037, 0.30729612708091736, 0.308440625667572, 0.30910825729370117, 0.30777302384376526, 0.3087267577648163, 0.30634239315986633, 0.3087267577648163, 0.3078683912754059, 0.3078683912754059, 0.307486891746521, 0.3088221251964569, 0.3088221251964569, 0.30948975682258606, 0.30901288986206055, 0.30910825729370117, 0.3083452582359314, 0.30805912613868713, 0.30853599309921265, 0.30853599309921265, 0.30891749262809753, 0.308440625667572, 0.3088221251964569, 0.30910825729370117, 0.30901288986206055, 0.30891749262809753, 0.30910825729370117, 0.30853599309921265, 0.3079637587070465, 0.3095851242542267, 0.3088221251964569, 0.30815449357032776, 0.3099666237831116, 0.3101573586463928, 0.3092989921569824, 0.31025275588035583, 0.31063422560691833, 0.3099666237831116, 0.3099666237831116, 0.3109203577041626, 0.3101573586463928, 0.31063422560691833, 0.31063422560691833, 0.310824990272522, 0.3109203577041626, 0.30939435958862305, 0.30948975682258606, 0.3078683912754059, 0.31111112236976624, 0.31063422560691833, 0.3104434907436371, 0.31120648980140686, 0.3087267577648163, 0.30987125635147095, 0.3101573586463928, 0.30910825729370117, 0.31034812331199646, 0.31063422560691833, 0.3100619912147522, 0.3092989921569824, 0.31025275588035583, 0.3105388581752777, 0.310824990272522, 0.31063422560691833, 0.31072962284088135, 0.30739152431488037, 0.30824989080429077, 0.3057701587677002, 0.3100619912147522, 0.3058655261993408, 0.30605626106262207, 0.30462566018104553, 0.30901288986206055, 0.30643776059150696, 0.30891749262809753, 0.30939435958862305, 0.3092036247253418, 0.3092989921569824, 0.30939435958862305, 0.30939435958862305, 0.30863139033317566, 0.30987125635147095, 0.30891749262809753, 0.3095851242542267, 0.3104434907436371, 0.30977585911750793, 0.3104434907436371, 0.31072962284088135, 0.3110157251358032, 0.30987125635147095, 0.31072962284088135, 0.31063422560691833, 0.3104434907436371, 0.3114926218986511, 0.3110157251358032, 0.31120648980140686, 0.3110157251358032, 0.31063422560691833, 0.3100619912147522, 0.31025275588035583, 0.3104434907436371, 0.3105388581752777, 0.3104434907436371, 0.31063422560691833, 0.3099666237831116, 0.31072962284088135, 0.3109203577041626, 0.3104434907436371, 0.31120648980140686, 0.31072962284088135, 0.3113972246646881, 0.3116833567619324, 0.3104434907436371, 0.3100619912147522, 0.311778724193573, 0.3110157251358032, 0.31063422560691833, 0.3122555911540985, 0.31025275588035583, 0.3113972246646881, 0.3110157251358032, 0.3104434907436371, 0.3122555911540985, 0.3110157251358032, 0.31244635581970215, 0.3125417232513428, 0.310824990272522, 0.31206485629081726, 0.3105388581752777, 0.3134000897407532, 0.31244635581970215, 0.3101573586463928, 0.3110157251358032, 0.31120648980140686, 0.3138769567012787, 0.31063422560691833, 0.3110157251358032, 0.3099666237831116, 0.3092036247253418, 0.311778724193573, 0.31072962284088135, 0.3139723539352417, 0.31206485629081726, 0.3118740916252136, 0.3113018572330475, 0.3122555911540985, 0.3126370906829834, 0.30910825729370117, 0.31330472230911255, 0.31368622183799744, 0.310824990272522, 0.3113018572330475, 0.3118740916252136, 0.3130185902118683, 0.31292322278022766, 0.3126370906829834, 0.3135908544063568, 0.31072962284088135, 0.3127324879169464, 0.3092036247253418, 0.31502145528793335, 0.315116822719574, 0.3104434907436371, 0.3134000897407532, 0.31282785534858704, 0.31025275588035583, 0.3114926218986511, 0.3142584562301636, 0.3109203577041626, 0.3140677213668823, 0.3140677213668823, 0.31072962284088135, 0.3140677213668823, 0.31540295481681824, 0.311778724193573, 0.3159751892089844, 0.31587982177734375, 0.31244635581970215, 0.3153075873851776, 0.31549832224845886, 0.31635668873786926, 0.31454458832740784, 0.3169289529323578, 0.3147353231906891, 0.3165474534034729, 0.31721505522727966, 0.3131139576435089, 0.3131139576435089, 0.3070100247859955, 0.29909393191337585, 0.3104434907436371, 0.30910825729370117, 0.3177873194217682, 0.31893181800842285, 0.31196948885917664, 0.31416308879852295, 0.3156890869140625, 0.31416308879852295, 0.3134954571723938, 0.31454458832740784, 0.31587982177734375, 0.3157844543457031, 0.3149260878562927, 0.31330472230911255, 0.3159751892089844, 0.3187410533428192, 0.3149260878562927, 0.3170243203639984, 0.3187410533428192, 0.31845492124557495, 0.31502145528793335, 0.31797805428504944, 0.3156890869140625, 0.31463995575904846, 0.30729612708091736, 0.2967095971107483, 0.310824990272522, 0.3130185902118683, 0.31711968779563904, 0.31540295481681824, 0.3127324879169464, 0.31196948885917664, 0.31683358550071716, 0.3178826868534088, 0.31416308879852295, 0.3138769567012787, 0.3149260878562927, 0.3139723539352417, 0.3147353231906891, 0.31769195199012756, 0.31807345151901245, 0.31502145528793335, 0.3164520859718323, 0.3192179203033447, 0.31845492124557495, 0.32112541794776917, 0.32226991653442383, 0.3183595538139343, 0.3195994198322296, 0.31330472230911255, 0.3048163950443268, 0.3088221251964569, 0.3186456859111786, 0.3071053922176361, 0.31463995575904846, 0.3164520859718323, 0.31721505522727966, 0.31769195199012756, 0.3153075873851776, 0.3191225528717041, 0.3203624188899994, 0.3153075873851776, 0.31940868496894836, 0.3234144151210785, 0.31711968779563904, 0.31797805428504944, 0.32064855098724365, 0.3190271854400635, 0.3199809193611145, 0.3233190178871155, 0.3190271854400635, 0.3243681490421295, 0.3216022849082947, 0.3198855519294739, 0.32064855098724365, 0.3216976523399353, 0.32370051741600037, 0.3212207853794098, 0.3198855519294739, 0.31206485629081726, 0.2980448305606842, 0.3175011873245239, 0.3242727816104889, 0.3148307204246521, 0.3170243203639984, 0.31979018449783325, 0.316165953874588, 0.3235097825527191, 0.3178826868534088, 0.32370051741600037, 0.3216022849082947, 0.3216976523399353, 0.32579874992370605, 0.3209346830844879, 0.320553183555603, 0.323891282081604, 0.3246542811393738, 0.32398664951324463, 0.32360514998435974, 0.32198378443717957, 0.3209346830844879, 0.3198855519294739, 0.3138769567012787, 0.3148307204246521, 0.30901288986206055, 0.32665711641311646, 0.315212219953537, 0.3174058198928833, 0.32236528396606445, 0.32284215092658997, 0.3255126476287842, 0.3220791518688202, 0.3250357508659363, 0.3255126476287842, 0.3203624188899994, 0.3243681490421295, 0.3195994198322296, 0.3256080150604248, 0.3264663815498352, 0.3233190178871155, 0.3259895145893097, 0.32370051741600037, 0.32017168402671814, 0.31759655475616455, 0.3140677213668823, 0.32446351647377014, 0.32284215092658997, 0.32589414715766907, 0.32226991653442383, 0.323795884847641, 0.32627564668655396, 0.3233190178871155, 0.32455888390541077, 0.3235097825527191, 0.32665711641311646, 0.32656174898147583, 0.32045778632164, 0.31845492124557495, 0.3247496485710144, 0.3268478810787201, 0.3224606513977051, 0.31940868496894836, 0.32064855098724365, 0.3192179203033447, 0.3243681490421295, 0.32446351647377014, 0.3255126476287842, 0.3243681490421295, 0.3285646140575409, 0.3233190178871155, 0.32761088013648987, 0.3252265155315399, 0.3247496485710144, 0.32713401317596436, 0.32532188296318054, 0.32627564668655396, 0.328183114528656, 0.3306628465652466, 0.32799237966537476, 0.3251311480998993, 0.30853599309921265, 0.30863139033317566, 0.3214115500450134, 0.31463995575904846, 0.31368622183799744, 0.32541725039482117, 0.3116833567619324, 0.32827848196029663, 0.3203624188899994, 0.32675251364707947, 0.32618024945259094, 0.32188841700553894, 0.32360514998435974, 0.32665711641311646, 0.32494038343429565, 0.32579874992370605, 0.3243681490421295, 0.32761088013648987, 0.3256080150604248, 0.328183114528656, 0.3277062475681305, 0.32751551270484924, 0.32408201694488525, 0.32923224568367004, 0.32913684844970703, 0.3298044800758362, 0.3256080150604248, 0.32322365045547485, 0.3250357508659363, 0.33190271258354187, 0.3306628465652466, 0.3273247480392456, 0.32484501600265503, 0.32589414715766907, 0.33190271258354187, 0.3303767144680023, 0.32913684844970703, 0.32846924662590027, 0.32665711641311646, 0.32322365045547485, 0.32837387919425964, 0.3323795795440674, 0.3298044800758362, 0.3260848820209503, 0.32742011547088623, 0.3277062475681305, 0.33304721117019653, 0.33228421211242676, 0.32789698243141174, 0.32837387919425964, 0.32703861594200134, 0.3311397135257721, 0.3324749767780304, 0.32589414715766907, 0.31626132130622864, 0.3246542811393738, 0.3298044800758362, 0.32627564668655396, 0.3199809193611145, 0.320553183555603, 0.319504052400589, 0.32789698243141174, 0.328183114528656, 0.3299952447414398, 0.3278016149997711, 0.33314257860183716, 0.3329518437385559, 0.32742011547088623, 0.33047211170196533, 0.33218884468078613, 0.33361944556236267, 0.33390557765960693, 0.32713401317596436, 0.33094897866249084, 0.3277062475681305, 0.3256080150604248, 0.3308536112308502, 0.3334287106990814, 0.3334287106990814, 0.32799237966537476, 0.3181688189506531, 0.33228421211242676, 0.3317119777202606, 0.3332379460334778, 0.3299952447414398, 0.328183114528656, 0.3298998475074768, 0.3332379460334778, 0.3334287106990814, 0.3334287106990814, 0.3289461135864258, 0.33047211170196533, 0.3354315757751465, 0.3337148427963257, 0.33524081110954285, 0.33390557765960693, 0.33657607436180115, 0.3311397135257721, 0.3324749767780304, 0.3241773843765259, 0.3110157251358032, 0.33409634232521057, 0.32656174898147583, 0.3316165804862976, 0.32923224568367004, 0.32970911264419556, 0.3277062475681305, 0.332570344209671, 0.33361944556236267, 0.3319980800151825, 0.331521213054657, 0.3332379460334778, 0.33266571164131165, 0.33133047819137573, 0.33476394414901733, 0.3341917097568512, 0.33733904361724854, 0.33476394414901733, 0.33266571164131165, 0.3355269432067871, 0.33485931158065796, 0.3334287106990814, 0.3319980800151825, 0.32656174898147583, 0.3286599814891815, 0.3362899422645569, 0.3329518437385559, 0.3320934772491455, 0.3341917097568512, 0.3312351107597351, 0.33619457483291626, 0.3342870771884918, 0.3329518437385559, 0.3345732092857361, 0.33094897866249084, 0.33657607436180115, 0.33619457483291626, 0.3303767144680023, 0.3159751892089844, 0.3333333432674408, 0.331521213054657, 0.33276107907295227, 0.3255126476287842, 0.32742011547088623, 0.32837387919425964, 0.3332379460334778, 0.3375298082828522, 0.33743444085121155, 0.33438244462013245, 0.3376251757144928, 0.3366714417934418, 0.3351454436779022, 0.32713401317596436, 0.33190271258354187, 0.3380066752433777, 0.3380066752433777, 0.3285646140575409, 0.33695754408836365, 0.3354315757751465, 0.33829280734062195, 0.33705294132232666, 0.3316165804862976, 0.33705294132232666, 0.33609917759895325, 0.3355269432067871, 0.3371483087539673, 0.33476394414901733, 0.3409632742404938, 0.3383881747722626, 0.3367668092250824, 0.34000954031944275, 0.3399141728878021, 0.3406771719455719, 0.3410586416721344, 0.3410586416721344, 0.34134477376937866, 0.33876967430114746, 0.3380066752433777, 0.3376251757144928, 0.3407725393772125, 0.3420124053955078, 0.3428707718849182, 0.3424892723560333, 0.34210777282714844, 0.33781594038009644, 0.34210777282714844, 0.33791130781173706, 0.3428707718849182, 0.33953267335891724, 0.34391987323760986, 0.3428707718849182, 0.34430137276649475, 0.3416309058666229, 0.343538373708725, 0.34000954031944275, 0.3440152704715729, 0.3323795795440674, 0.31797805428504944, 0.3337148427963257, 0.3409632742404938, 0.33867430686950684, 0.32875537872314453, 0.3269432485103607, 0.33361944556236267, 0.3332379460334778, 0.3362899422645569, 0.3441106379032135, 0.3381020426750183, 0.34134477376937866, 0.34172627329826355, 0.3397234082221985, 0.3422985076904297, 0.33962804079055786, 0.3428707718849182, 0.3424892723560333, 0.34515973925590515, 0.3405817747116089, 0.34649500250816345, 0.3454458713531494, 0.3454458713531494, 0.34172627329826355, 0.3450643718242645, 0.3394373059272766, 0.34430137276649475, 0.34172627329826355, 0.3442060053348541, 0.34124940633773804, 0.3487839698791504, 0.34649500250816345, 0.3449690043926239, 0.34687650203704834, 0.3458273708820343, 0.34515973925590515, 0.34048640727996826, 0.3268478810787201, 0.33352407813072205, 0.3474487364292145]</t>
+  </si>
+  <si>
+    <t>[0.2407248467206955, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.2735336124897003, 0.27448737621307373, 0.29566046595573425, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30548402667045593, 0.30815449357032776, 0.3078683912754059, 0.3083452582359314, 0.3058655261993408, 0.3065331280231476, 0.3067238926887512, 0.30805912613868713, 0.30739152431488037, 0.30729612708091736, 0.308440625667572, 0.30910825729370117, 0.30777302384376526, 0.3087267577648163, 0.30634239315986633, 0.3087267577648163, 0.3078683912754059, 0.3078683912754059, 0.307486891746521, 0.3088221251964569, 0.3088221251964569, 0.30948975682258606, 0.30901288986206055, 0.30910825729370117, 0.3083452582359314, 0.30805912613868713, 0.30853599309921265, 0.30853599309921265, 0.30891749262809753, 0.308440625667572, 0.3088221251964569, 0.30910825729370117, 0.30901288986206055, 0.30891749262809753, 0.30910825729370117, 0.30853599309921265, 0.3079637587070465, 0.3095851242542267, 0.3088221251964569, 0.30815449357032776, 0.3099666237831116, 0.3101573586463928, 0.3092989921569824, 0.31025275588035583, 0.31063422560691833, 0.3099666237831116, 0.3099666237831116, 0.30557939410209656, 0.28068670630455017, 0.26857414841651917, 0.25436338782310486, 0.25007152557373047, 0.25178825855255127, 0.2588459849357605, 0.27057701349258423, 0.3061516582965851, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.3066285252571106, 0.30643776059150696, 0.30805912613868713, 0.30777302384376526, 0.30853599309921265, 0.30891749262809753, 0.3092989921569824, 0.30901288986206055, 0.3092989921569824, 0.3092036247253418, 0.30910825729370117, 0.3088221251964569, 0.30891749262809753, 0.3087267577648163, 0.30891749262809753, 0.30863139033317566, 0.3088221251964569, 0.30910825729370117, 0.30901288986206055, 0.30863139033317566, 0.308440625667572, 0.308440625667572, 0.30891749262809753, 0.3092036247253418, 0.30977585911750793, 0.30987125635147095, 0.30987125635147095, 0.3104434907436371, 0.31034812331199646, 0.31034812331199646, 0.3101573586463928, 0.31063422560691833, 0.31025275588035583, 0.31072962284088135, 0.3109203577041626, 0.31025275588035583, 0.3105388581752777, 0.3096804916858673, 0.31072962284088135, 0.30901288986206055, 0.31063422560691833, 0.3092036247253418, 0.31025275588035583, 0.31063422560691833, 0.3105388581752777, 0.3099666237831116, 0.31111112236976624, 0.30948975682258606, 0.3104434907436371, 0.30977585911750793, 0.3096804916858673, 0.3071053922176361, 0.3096804916858673, 0.31025275588035583, 0.30901288986206055, 0.31111112236976624, 0.30939435958862305, 0.30891749262809753, 0.310824990272522, 0.31025275588035583, 0.310824990272522, 0.3095851242542267, 0.30939435958862305, 0.3088221251964569, 0.30977585911750793, 0.31034812331199646, 0.30948975682258606, 0.22708632051944733, 0.278969943523407, 0.30863139033317566, 0.3056747615337372, 0.30557939410209656, 0.2937529683113098, 0.2979494631290436, 0.30805912613868713, 0.30729612708091736, 0.30805912613868713, 0.3071053922176361, 0.3065331280231476, 0.30596089363098145, 0.30557939410209656, 0.30557939410209656, 0.30557939410209656, 0.3053886592388153, 0.3078683912754059, 0.30863139033317566, 0.3092036247253418, 0.30910825729370117, 0.30901288986206055, 0.3095851242542267, 0.3096804916858673, 0.30977585911750793, 0.3099666237831116, 0.30948975682258606, 0.3095851242542267, 0.3092989921569824, 0.30987125635147095, 0.30977585911750793, 0.3092989921569824, 0.31025275588035583, 0.31025275588035583, 0.3096804916858673, 0.30948975682258606, 0.30977585911750793, 0.3101573586463928, 0.3096804916858673, 0.30948975682258606, 0.3096804916858673, 0.30948975682258606, 0.30939435958862305, 0.3104434907436371, 0.3101573586463928, 0.3099666237831116, 0.3101573586463928, 0.30987125635147095, 0.30987125635147095, 0.30977585911750793, 0.3099666237831116, 0.31034812331199646, 0.30977585911750793, 0.3101573586463928, 0.3101573586463928, 0.30939435958862305, 0.3096804916858673, 0.30987125635147095, 0.30977585911750793, 0.3099666237831116, 0.3095851242542267, 0.3096804916858673, 0.3095851242542267, 0.3100619912147522, 0.31034812331199646, 0.3101573586463928, 0.3100619912147522, 0.3100619912147522, 0.30977585911750793, 0.3101573586463928, 0.30987125635147095, 0.31025275588035583, 0.3109203577041626, 0.3105388581752777, 0.3114926218986511, 0.3104434907436371, 0.3122555911540985, 0.3105388581752777, 0.3105388581752777, 0.3113972246646881, 0.30987125635147095, 0.3113018572330475, 0.3101573586463928, 0.3114926218986511, 0.3122555911540985, 0.3100619912147522, 0.3122555911540985, 0.3121602237224579, 0.3100619912147522, 0.3123509883880615, 0.3134000897407532, 0.31072962284088135, 0.3113972246646881, 0.3130185902118683, 0.3121602237224579, 0.31196948885917664, 0.31196948885917664, 0.3125417232513428, 0.31330472230911255, 0.3101573586463928, 0.31378158926963806, 0.3139723539352417, 0.3118740916252136, 0.3125417232513428, 0.3135908544063568, 0.31196948885917664, 0.3134000897407532, 0.31206485629081726, 0.3130185902118683, 0.31502145528793335, 0.31072962284088135, 0.3132093548774719, 0.3130185902118683, 0.31282785534858704, 0.31416308879852295, 0.3132093548774719, 0.3153075873851776, 0.3118740916252136, 0.3144492208957672, 0.3116833567619324, 0.31549832224845886, 0.31587982177734375, 0.31196948885917664, 0.3140677213668823, 0.3138769567012787, 0.3125417232513428, 0.30901288986206055, 0.3134000897407532, 0.31158798933029175, 0.3104434907436371, 0.31378158926963806, 0.31063422560691833, 0.3125417232513428, 0.3147353231906891, 0.3144492208957672, 0.3126370906829834, 0.3147353231906891, 0.3156890869140625, 0.31416308879852295, 0.3143538534641266, 0.3174058198928833, 0.3138769567012787, 0.3132093548774719, 0.31587982177734375, 0.3156890869140625, 0.3153075873851776, 0.31587982177734375, 0.3156890869140625, 0.31626132130622864, 0.31683358550071716, 0.3157844543457031, 0.3155937194824219, 0.3174058198928833, 0.3156890869140625, 0.316165953874588, 0.31587982177734375, 0.31673818826675415, 0.31368622183799744, 0.3142584562301636, 0.31759655475616455, 0.3186456859111786, 0.31454458832740784, 0.31807345151901245, 0.316165953874588, 0.31549832224845886, 0.31721505522727966, 0.3169289529323578, 0.3174058198928833, 0.3177873194217682, 0.3174058198928833, 0.3198855519294739, 0.31759655475616455, 0.31845492124557495, 0.3203624188899994, 0.3181688189506531, 0.3200762867927551, 0.3135908544063568, 0.30205056071281433, 0.315116822719574, 0.3169289529323578, 0.3199809193611145, 0.31549832224845886, 0.3186456859111786, 0.31797805428504944, 0.3191225528717041, 0.3213161528110504, 0.3183595538139343, 0.3183595538139343, 0.31979018449783325, 0.3187410533428192, 0.3207439184188843, 0.32017168402671814, 0.3225560188293457, 0.3198855519294739, 0.31759655475616455, 0.3096804916858673, 0.3092989921569824, 0.3177873194217682, 0.31855031847953796, 0.3132093548774719, 0.3153075873851776, 0.32112541794776917, 0.3217930495738983, 0.3155937194824219, 0.3221745491027832, 0.31893181800842285, 0.3173104524612427, 0.3187410533428192, 0.3187410533428192, 0.32112541794776917, 0.31893181800842285, 0.3220791518688202, 0.3200762867927551, 0.3216022849082947, 0.3234144151210785, 0.3243681490421295, 0.3225560188293457, 0.32064855098724365, 0.3181688189506531, 0.3198855519294739, 0.32026705145835876, 0.31797805428504944, 0.3187410533428192, 0.32446351647377014, 0.3233190178871155, 0.32188841700553894, 0.3241773843765259, 0.32103005051612854, 0.3178826868534088, 0.3224606513977051, 0.32408201694488525, 0.32446351647377014, 0.3203624188899994, 0.31979018449783325, 0.3192179203033447, 0.3234144151210785, 0.3247496485710144, 0.3229375183582306, 0.3186456859111786, 0.3166428208351135, 0.3192179203033447, 0.3246542811393738, 0.3256080150604248, 0.32103005051612854, 0.3198855519294739, 0.3220791518688202, 0.32799237966537476, 0.3246542811393738, 0.32322365045547485, 0.31673818826675415, 0.3203624188899994, 0.323795884847641, 0.3263710141181946, 0.3220791518688202, 0.32103005051612854, 0.32274678349494934, 0.32656174898147583, 0.3252265155315399, 0.32570338249206543, 0.3255126476287842, 0.32226991653442383, 0.32198378443717957, 0.3251311480998993, 0.3260848820209503, 0.32494038343429565, 0.3260848820209503, 0.327229380607605, 0.3268478810787201, 0.3277062475681305, 0.3252265155315399, 0.32236528396606445, 0.30176442861557007, 0.30548402667045593, 0.323795884847641, 0.30824989080429077, 0.31979018449783325, 0.3153075873851776, 0.3252265155315399, 0.31807345151901245, 0.323891282081604, 0.31931331753730774, 0.3246542811393738, 0.3229375183582306, 0.32532188296318054, 0.31940868496894836, 0.3220791518688202, 0.3247496485710144, 0.32627564668655396, 0.3277062475681305, 0.3260848820209503, 0.32751551270484924, 0.32446351647377014, 0.3280877470970154, 0.3247496485710144, 0.327229380607605, 0.32875537872314453, 0.32703861594200134, 0.32713401317596436, 0.32398664951324463, 0.31769195199012756, 0.3138769567012787, 0.3259895145893097, 0.323891282081604, 0.3213161528110504, 0.3241773843765259, 0.32618024945259094, 0.3208392858505249, 0.3273247480392456, 0.32589414715766907, 0.32274678349494934, 0.3285646140575409, 0.32799237966537476, 0.32875537872314453, 0.32837387919425964, 0.3285646140575409, 0.3302813470363617, 0.3259895145893097, 0.32656174898147583, 0.32846924662590027, 0.3269432485103607, 0.3273247480392456, 0.32751551270484924, 0.3295183479785919, 0.3303767144680023, 0.33190271258354187, 0.3317119777202606, 0.3295183479785919, 0.331521213054657, 0.32656174898147583, 0.30987125635147095, 0.31587982177734375, 0.32827848196029663, 0.32284215092658997, 0.3214115500450134, 0.3290414810180664, 0.3264663815498352, 0.32665711641311646, 0.32751551270484924, 0.32398664951324463, 0.3307582139968872, 0.32827848196029663, 0.33018597960472107, 0.3320934772491455, 0.3319980800151825, 0.3337148427963257, 0.33218884468078613, 0.33409634232521057, 0.33218884468078613, 0.3333333432674408, 0.3307582139968872, 0.33409634232521057, 0.331521213054657, 0.32961374521255493, 0.3234144151210785, 0.3126370906829834, 0.32360514998435974, 0.33047211170196533, 0.3216022849082947, 0.32312828302383423, 0.32761088013648987, 0.32484501600265503, 0.32923224568367004, 0.33276107907295227, 0.32961374521255493, 0.3295183479785919, 0.33190271258354187, 0.3329518437385559, 0.33228421211242676, 0.33228421211242676, 0.3341917097568512, 0.33190271258354187, 0.33533620834350586, 0.33476394414901733, 0.33180734515190125, 0.33476394414901733, 0.33476394414901733, 0.3350500762462616, 0.33390557765960693, 0.3337148427963257, 0.33218884468078613, 0.3317119777202606]</t>
+  </si>
+  <si>
+    <t>[0.26589256525039673, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.30815401673316956, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081900179386139, 0.3081919848918915, 0.3081919848918915, 0.3081919848918915, 0.3081919848918915, 0.3081919848918915, 0.3081919848918915, 0.3081919848918915, 0.3081929385662079, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081929385662079, 0.3081939220428467, 0.3081929385662079, 0.3081939220428467, 0.3081929385662079, 0.3081929385662079, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081929385662079, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3090931177139282, 0.3081939220428467, 0.3081939220428467, 0.3095057010650635, 0.30821046233177185, 0.30978307127952576, 0.3081939220428467, 0.30836910009384155, 0.3085753917694092, 0.31005650758743286, 0.3090541660785675, 0.30865713953971863, 0.3097665011882782, 0.30827081203460693, 0.30858805775642395, 0.3082484304904938, 0.3073686957359314, 0.3086318373680115, 0.3083019554615021, 0.3086113929748535, 0.30827081203460693, 0.3081929385662079, 0.3071575164794922, 0.30870482325553894, 0.3081929385662079, 0.309207946062088, 0.3083574175834656, 0.3086688220500946, 0.30820658802986145, 0.3097188174724579, 0.3091203570365906, 0.3082231283187866, 0.31000882387161255, 0.30950766801834106, 0.3083963394165039, 0.30864351987838745, 0.3094288408756256, 0.3100234270095825, 0.30879825353622437, 0.30979570746421814, 0.30990374088287354, 0.3088741600513458, 0.3101440966129303, 0.3099163770675659, 0.3095397651195526, 0.3101421594619751, 0.30991053581237793, 0.3101041913032532, 0.30946969985961914, 0.3103173077106476, 0.31039223074913025, 0.3103640079498291, 0.31033191084861755, 0.31049734354019165, 0.30903178453445435, 0.309330552816391, 0.31055572628974915, 0.31093525886535645, 0.31130504608154297, 0.3097013235092163, 0.31012073159217834, 0.31074258685112, 0.31132256984710693, 0.31121259927749634, 0.3112194240093231, 0.3111950755119324, 0.3101401925086975, 0.309776246547699, 0.3090502917766571, 0.30838271975517273, 0.3109741806983948, 0.3100954294204712, 0.3097051978111267, 0.3111211359500885, 0.30885177850723267, 0.31097710132598877, 0.3111308515071869, 0.30978599190711975, 0.3111269772052765, 0.27761110663414, 0.2685852348804474, 0.29176053404808044, 0.3058837056159973, 0.28423622250556946, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081939220428467, 0.3081939220428467, 0.3081919848918915, 0.3081919848918915, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081919848918915, 0.3081919848918915, 0.3081919848918915, 0.3081919848918915, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081929385662079, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081929385662079, 0.3081929385662079, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.3081939220428467, 0.30836227536201477, 0.3089520037174225, 0.3090950548648834, 0.30931204557418823, 0.30973830819129944, 0.31021514534950256, 0.3106267750263214, 0.31083598732948303, 0.31093525886535645, 0.3110277056694031, 0.31103646755218506, 0.31092455983161926, 0.31110361218452454, 0.31131479144096375, 0.31154152750968933, 0.31175851821899414, 0.3121146857738495, 0.3120631277561188, 0.3123093247413635, 0.31202712655067444, 0.3127423822879791, 0.31169819831848145, 0.3124455511569977, 0.3114665746688843, 0.3128494322299957, 0.31245043873786926, 0.31225287914276123, 0.3130391836166382, 0.311730295419693, 0.3128056228160858, 0.3121711313724518, 0.31316277384757996, 0.3133165240287781, 0.31245043873786926, 0.3130323588848114, 0.3114617168903351, 0.31278908252716064, 0.31196191906929016, 0.3138420283794403, 0.3134644329547882, 0.3131977915763855, 0.3138634264469147, 0.3118227422237396, 0.3136230707168579, 0.31240859627723694, 0.3149338662624359, 0.3143967092037201, 0.3140570819377899, 0.31491246819496155, 0.3125866651535034, 0.31349265575408936, 0.3116777539253235, 0.3155245780944824, 0.3156968355178833, 0.31416022777557373, 0.31507790088653564, 0.31329023838043213, 0.31599265336990356, 0.3159109055995941, 0.3136308491230011, 0.3156442642211914, 0.31410086154937744, 0.31703585386276245, 0.3163624405860901, 0.31451737880706787, 0.31562772393226624, 0.3140697479248047, 0.3161259889602661, 0.3153679072856903, 0.31719741225242615, 0.31779003143310547, 0.3144482970237732, 0.3148881494998932, 0.3130985498428345, 0.31604716181755066, 0.31671667098999023, 0.3175594210624695, 0.3145942687988281, 0.3150448203086853, 0.3176761865615845, 0.3180566728115082, 0.31634005904197693, 0.31725093722343445, 0.31562870740890503, 0.31882935762405396, 0.31606757640838623, 0.3177725374698639, 0.31802359223365784, 0.31611430644989014, 0.3185870349407196, 0.318703830242157, 0.3189169466495514, 0.31904831528663635, 0.31877484917640686, 0.318692147731781, 0.3183028995990753, 0.3185374140739441, 0.31692785024642944, 0.31027936935424805, 0.3113507926464081, 0.3081413805484772, 0.3175594210624695, 0.31310731172561646, 0.31823572516441345, 0.3059946298599243, 0.3188128173351288, 0.311942458152771, 0.31539416313171387, 0.31823864579200745, 0.31786301732063293, 0.31599557399749756, 0.31899285316467285, 0.31835347414016724, 0.31692588329315186, 0.3158058226108551, 0.3187106251716614, 0.3183816969394684, 0.3178746998310089, 0.3191242218017578, 0.31949400901794434, 0.31833013892173767, 0.3194103240966797, 0.31906095147132874, 0.3191446363925934, 0.3196682035923004, 0.31991925835609436, 0.3193052113056183, 0.3199104964733124, 0.3202695846557617, 0.32008275389671326, 0.32042044401168823, 0.319446325302124, 0.32057321071624756, 0.31938305497169495, 0.3181510865688324, 0.31671959161758423, 0.3158554434776306, 0.31775596737861633, 0.32089143991470337, 0.3152530789375305, 0.3153669238090515, 0.3159294128417969, 0.3200623095035553, 0.317937970161438, 0.32014310359954834, 0.3186970055103302, 0.31834083795547485, 0.3195232152938843, 0.32045644521713257, 0.31910476088523865, 0.32074740529060364, 0.32007691264152527, 0.32030755281448364, 0.32023942470550537, 0.3210471272468567, 0.32063451409339905, 0.3209332823753357, 0.32035523653030396, 0.3214315176010132, 0.3209916651248932, 0.32105687260627747, 0.3209303617477417, 0.32107633352279663, 0.32106465101242065, 0.31931689381599426, 0.31441518664360046, 0.31709522008895874, 0.31964483857154846, 0.3193431794643402, 0.3183067739009857, 0.3200613558292389, 0.320229709148407, 0.3191845417022705, 0.3201771378517151, 0.32135269045829773, 0.3192409873008728, 0.3216923177242279, 0.3208135962486267, 0.3216942846775055, 0.3214772641658783, 0.3209877610206604, 0.322064071893692, 0.32182660698890686, 0.32188111543655396, 0.3219764828681946, 0.32091188430786133, 0.3222256004810333, 0.32138481736183167, 0.3222236633300781, 0.32172250747680664, 0.322306364774704, 0.3221769630908966, 0.32227036356925964, 0.32221588492393494, 0.32183828949928284, 0.3220767080783844, 0.32096245884895325, 0.3173852264881134, 0.29889947175979614, 0.3161357045173645, 0.3215774893760681, 0.310967355966568, 0.3175594210624695, 0.3156530261039734, 0.32089337706565857, 0.3212699890136719, 0.31626805663108826, 0.31746792793273926, 0.3211648762226105, 0.32144027948379517, 0.3178766369819641, 0.3200652301311493, 0.3206656575202942, 0.32133129239082336, 0.3194570243358612, 0.3210821747779846, 0.32121744751930237, 0.3206004798412323, 0.3213176727294922, 0.3214227557182312, 0.3217886686325073, 0.3213634192943573, 0.32200178503990173, 0.3224659860134125, 0.3214091360569, 0.32237547636032104, 0.3223968744277954, 0.3220231831073761, 0.32198524475097656, 0.32205337285995483, 0.32264599204063416, 0.3222333788871765, 0.32199692726135254, 0.32248055934906006, 0.32254868745803833, 0.32265961170196533, 0.32286691665649414, 0.32264599204063416, 0.3222285211086273, 0.3224056363105774, 0.3220718502998352, 0.3219638466835022, 0.3219550848007202, 0.32194435596466064, 0.32265767455101013, 0.3227676451206207, 0.322952538728714, 0.32315593957901, 0.3227277398109436, 0.32303136587142944, 0.32279977202415466, 0.32248055934906006, 0.32198232412338257, 0.32138481736183167, 0.32112985849380493, 0.3220134675502777, 0.3219151794910431, 0.32307711243629456, 0.32326003909111023, 0.3217516839504242, 0.3222470283508301, 0.3223384916782379, 0.32335445284843445, 0.323275625705719, 0.32291263341903687, 0.3231169879436493, 0.32303720712661743, 0.3227238655090332, 0.3224445581436157, 0.32254868745803833, 0.32255062460899353, 0.3230955898761749, 0.32264891266822815, 0.3231121301651001, 0.3225233852863312, 0.32330286502838135, 0.3235948085784912, 0.3235364258289337, 0.3234245181083679, 0.3226771354675293, 0.3225584328174591, 0.32176822423934937, 0.31942978501319885, 0.3202783465385437, 0.3208904564380646, 0.3232347369194031, 0.3215259313583374, 0.3226771354675293, 0.3222869038581848, 0.32184121012687683, 0.32231417298316956, 0.32286885380744934, 0.32232874631881714, 0.3221253752708435, 0.3233661353588104, 0.3228532671928406, 0.322512686252594, 0.32314619421958923, 0.3232260048389435, 0.32318997383117676, 0.3229943811893463, 0.32385367155075073, 0.3236570954322815, 0.3231705129146576, 0.324032723903656, 0.32389453053474426, 0.3234819173812866, 0.322309285402298, 0.32247960567474365, 0.3214218020439148, 0.32258760929107666, 0.32198816537857056, 0.3224503993988037, 0.323607474565506, 0.32323572039604187, 0.32258468866348267, 0.3231792747974396, 0.3243772089481354, 0.3231150507926941, 0.32324641942977905, 0.3243217468261719, 0.32384589314460754, 0.3237758278846741, 0.3238215446472168, 0.3244112730026245, 0.324358731508255, 0.3234751224517822, 0.323835164308548, 0.3232629597187042, 0.3234507739543915, 0.32290583848953247, 0.3218441307544708, 0.3217059373855591, 0.3230021595954895, 0.32297101616859436, 0.3235422670841217, 0.32427698373794556, 0.322180837392807, 0.324044406414032, 0.3240512013435364, 0.324041485786438, 0.32372909784317017, 0.32285717129707336, 0.32428380846977234, 0.3245338797569275, 0.32385268807411194, 0.32433438301086426, 0.324481338262558, 0.32429060339927673, 0.32379722595214844, 0.32410377264022827, 0.32444727420806885, 0.324598103761673, 0.3237106204032898, 0.3244141936302185, 0.3243596851825714, 0.3249484598636627, 0.3246175944805145, 0.32412418723106384, 0.32411348819732666, 0.32394805550575256, 0.32388773560523987, 0.3238205909729004, 0.3222976326942444, 0.3244677186012268, 0.3248997926712036, 0.3248024880886078, 0.32466331124305725, 0.3237116038799286, 0.3240512013435364, 0.32416799664497375, 0.32335737347602844, 0.32417967915534973, 0.3256744146347046, 0.32486864924430847, 0.32439863681793213, 0.32508954405784607, 0.32449886202812195, 0.3244687020778656, 0.3237135410308838, 0.3250662088394165, 0.32536301016807556, 0.3243188261985779, 0.32525497674942017, 0.3258271813392639, 0.32525402307510376, 0.325441837310791, 0.3252287209033966, 0.3254992365837097, 0.32527443766593933, 0.3237699866294861, 0.3207688331604004, 0.32219642400741577, 0.32508760690689087, 0.32499125599861145, 0.32214775681495667, 0.3240200877189636, 0.3253532648086548, 0.3226158320903778, 0.3242380619049072, 0.3250253200531006, 0.3246993124485016, 0.3233709931373596, 0.3251751959323883, 0.3240872323513031, 0.32450857758522034, 0.3249484598636627, 0.3251761496067047, 0.3246428966522217, 0.3255012035369873, 0.3259274363517761, 0.32613080739974976, 0.325558602809906, 0.3265395164489746, 0.32586902379989624, 0.325989693403244, 0.32591575384140015, 0.32603156566619873, 0.32657942175865173, 0.32694143056869507, 0.325887531042099, 0.3259546756744385, 0.32618433237075806, 0.3252491354942322, 0.325687050819397, 0.3263731300830841, 0.3267088532447815, 0.3255099356174469, 0.3245786428451538, 0.3254515528678894, 0.32641106843948364, 0.32601112127304077, 0.32532504200935364, 0.3264947533607483, 0.32635462284088135, 0.3270387351512909, 0.3256111443042755, 0.3262086510658264, 0.32683828473091125, 0.3274241089820862, 0.3267166316509247, 0.32590892910957336, 0.325681209564209, 0.3265463411808014, 0.3259848356246948, 0.3256033658981323, 0.3274562358856201, 0.3263089060783386, 0.32749903202056885, 0.32744941115379333, 0.32608312368392944, 0.3260938227176666, 0.3264869749546051, 0.32712438702583313, 0.3266952335834503, 0.32760512828826904, 0.32819971442222595, 0.32628652453422546, 0.3266962170600891, 0.32661542296409607, 0.3262777626514435, 0.32662224769592285, 0.32661446928977966, 0.32521897554397583, 0.327422171831131, 0.32748445868492126, 0.32760706543922424, 0.32732194662094116, 0.3264431953430176, 0.32672637701034546, 0.32635462284088135, 0.327075719833374, 0.32792916893959045, 0.32797977328300476, 0.32754576206207275, 0.32830771803855896, 0.32771703600883484, 0.32695117592811584, 0.3265327215194702, 0.3264986574649811, 0.3270397186279297, 0.32776957750320435, 0.3283427655696869, 0.32843032479286194, 0.3267594575881958, 0.32716330885887146, 0.3276401460170746, 0.32809266448020935, 0.32858797907829285, 0.3279661536216736, 0.328511118888855, 0.3284887373447418, 0.3277014493942261, 0.3265482783317566, 0.3268042206764221, 0.32739686965942383, 0.3288303017616272, 0.32864540815353394, 0.3277014493942261, 0.32672929763793945, 0.3285500407218933, 0.32901617884635925, 0.32738032937049866, 0.3275856673717499, 0.3288332223892212, 0.3285042941570282, 0.3281627297401428, 0.3279719948768616, 0.3284585475921631, 0.329050213098526, 0.3277871012687683, 0.32400158047676086, 0.32668548822402954, 0.32842060923576355, 0.32826295495033264, 0.3257687985897064, 0.32891204953193665, 0.32799047231674194, 0.3282308578491211, 0.3277374505996704, 0.32775983214378357, 0.3285101354122162, 0.3289324641227722, 0.3289967179298401, 0.32781240344047546, 0.32787662744522095, 0.3285655975341797, 0.3288322389125824, 0.32924193143844604, 0.32857629656791687, 0.3296370208263397, 0.3298151195049286, 0.3281238079071045, 0.3281257450580597, 0.32941222190856934, 0.32837098836898804, 0.328619122505188, 0.3274036645889282, 0.32373687624931335, 0.3281062841415405, 0.3269326686859131, 0.326315701007843, 0.32498931884765625, 0.32515281438827515, 0.3279554545879364, 0.3277267515659332, 0.3272518813610077, 0.32743188738822937, 0.3282785415649414, 0.3273637890815735, 0.3279972970485687, 0.3285013735294342, 0.3281773328781128, 0.3284546732902527, 0.32902491092681885, 0.3283923864364624, 0.3263234794139862, 0.3285655975341797, 0.3294813334941864, 0.32919618487358093, 0.3294998109340668, 0.32885852456092834, 0.3289490342140198, 0.33037465810775757, 0.32930228114128113, 0.32984721660614014, 0.32999610900878906, 0.33011290431022644, 0.3297956585884094, 0.33033186197280884, 0.3302997350692749, 0.329818993806839, 0.3301995098590851, 0.32701441645622253, 0.3183729648590088, 0.32699787616729736, 0.3239344358444214, 0.3259906768798828, 0.32655802369117737, 0.3227384388446808, 0.3280148208141327, 0.32673317193984985, 0.3298511207103729, 0.3268596827983856, 0.33006131649017334, 0.329710990190506, 0.329576700925827, 0.3293324410915375, 0.3290570378303528, 0.32969930768013, 0.33010706305503845, 0.33022284507751465, 0.3304067850112915, 0.33011874556541443, 0.3295494318008423, 0.3308407962322235, 0.3300204575061798, 0.3295523524284363, 0.3304758667945862, 0.33120086789131165, 0.33059558272361755, 0.3306238055229187, 0.3306802213191986, 0.3309546709060669, 0.3297693729400635, 0.329262375831604, 0.32783281803131104, 0.33082035183906555, 0.3305303752422333, 0.3291524052619934, 0.3307249844074249, 0.3294745087623596, 0.33028319478034973, 0.3318333923816681, 0.3308008909225464, 0.3316027820110321, 0.3311288356781006, 0.3316066563129425, 0.33032989501953125, 0.33108505606651306, 0.3306228220462799, 0.3318898379802704, 0.33146554231643677, 0.3310548961162567, 0.33228492736816406, 0.3315472900867462, 0.3316017985343933, 0.3319297432899475, 0.331883043050766, 0.332433819770813, 0.3325885534286499, 0.3298063576221466, 0.31947553157806396, 0.326973557472229, 0.3276323676109314, 0.3278902471065521, 0.3280148208141327, 0.3232191801071167, 0.329708069562912, 0.3270300030708313, 0.3301498591899872, 0.3302549719810486, 0.3296000361442566, 0.33069679141044617, 0.3293207585811615, 0.33022090792655945, 0.33036008477211, 0.33102765679359436, 0.3310772776603699, 0.33145973086357117, 0.3312874734401703, 0.33038732409477234, 0.33163389563560486, 0.3308388590812683, 0.3324854075908661, 0.3313215374946594, 0.33239394426345825, 0.33125340938568115, 0.3317068815231323, 0.33104419708251953, 0.3314869701862335, 0.3306179642677307, 0.33235305547714233, 0.3327432870864868, 0.3318791389465332, 0.3329612612724304, 0.3318976163864136, 0.3310811519622803, 0.3303649425506592, 0.3312699496746063, 0.33167770504951477, 0.3335237503051758, 0.33284351229667664, 0.3313799202442169, 0.33273744583129883, 0.3321983218193054, 0.3335655927658081, 0.33272868394851685, 0.3338584899902344, 0.333511084318161, 0.33342641592025757, 0.33396750688552856, 0.33251556754112244, 0.33142662048339844, 0.33026859164237976, 0.33202511072158813, 0.3323131501674652, 0.33251655101776123, 0.3333660960197449, 0.3302919566631317, 0.3331899642944336, 0.3327968120574951, 0.3324202001094818, 0.33342352509498596, 0.3323715627193451, 0.33288049697875977, 0.3311619460582733, 0.33337193727493286, 0.33403465151786804, 0.3327072858810425, 0.3335821330547333, 0.3319278061389923, 0.3338468372821808, 0.33202219009399414, 0.33343616127967834, 0.3337242007255554, 0.3334050178527832, 0.3341192901134491, 0.3326012194156647, 0.3335247039794922, 0.3319929838180542, 0.3337427079677582, 0.3329710066318512, 0.33495813608169556, 0.33446964621543884, 0.33453190326690674, 0.33425456285476685, 0.3345562517642975, 0.3340725898742676, 0.3311814069747925, 0.33026567101478577, 0.3312767744064331, 0.33327850699424744, 0.3332892060279846, 0.3308544158935547, 0.33327266573905945, 0.3320455551147461, 0.3346214294433594, 0.3329330384731293, 0.33114635944366455, 0.33223336935043335, 0.33136922121047974, 0.3316057026386261, 0.3313896656036377, 0.32864734530448914, 0.333065390586853, 0.3294793665409088, 0.3299241065979004, 0.3296506404876709, 0.3330877721309662, 0.3318275511264801, 0.3343781530857086, 0.331880122423172, 0.3328114151954651, 0.3328104317188263, 0.3332318067550659, 0.333071231842041, 0.3340015411376953, 0.3334069550037384, 0.33344393968582153, 0.334809273481369, 0.33408036828041077, 0.33544665575027466, 0.333732008934021, 0.3347674012184143, 0.3353824317455292, 0.3338584899902344, 0.3356364369392395, 0.3347557485103607, 0.33543694019317627, 0.3337378203868866, 0.3354125916957855, 0.3347567021846771, 0.33528706431388855, 0.3351021707057953, 0.33604806661605835, 0.33616483211517334, 0.33556053042411804, 0.3361774981021881, 0.3345017433166504, 0.3341582417488098, 0.3311716616153717, 0.3331851065158844, 0.3348102271556854, 0.3312845528125763, 0.33424872159957886, 0.3342273235321045, 0.3327121436595917, 0.33474892377853394, 0.33430713415145874, 0.33440929651260376, 0.33431586623191833, 0.33545249700546265, 0.3349863588809967, 0.33578044176101685, 0.3340035080909729, 0.3367341160774231, 0.33654046058654785, 0.33322304487228394, 0.3366085886955261, 0.33660373091697693, 0.3363477885723114, 0.33687230944633484, 0.33508172631263733, 0.33686161041259766, 0.33571428060531616, 0.3370474874973297, 0.33723723888397217, 0.3363361060619354, 0.33632931113243103, 0.33468955755233765, 0.3348335921764374, 0.3324299454689026, 0.3341698944568634, 0.33299338817596436, 0.33130109310150146, 0.3349854052066803, 0.3346710801124573, 0.33300700783729553, 0.33529776334762573, 0.33327072858810425, 0.3339042365550995, 0.3341270983219147, 0.334494948387146, 0.33484235405921936, 0.33630886673927307, 0.336026668548584, 0.33616289496421814, 0.33674484491348267, 0.33614635467529297, 0.336559921503067, 0.33670881390571594, 0.3370036780834198, 0.33750680088996887, 0.3372051417827606, 0.33740168809890747, 0.33681976795196533, 0.33780360221862793, 0.337866872549057, 0.33816075325012207, 0.3366786539554596, 0.3318207561969757, 0.33054301142692566, 0.32977619767189026, 0.3349415957927704, 0.33191418647766113, 0.3348909914493561, 0.33790189027786255, 0.33293402194976807, 0.3364178538322449, 0.3362232446670532, 0.3353532552719116, 0.3369083106517792, 0.33768975734710693, 0.3370484411716461, 0.33736473321914673, 0.3378026485443115, 0.3377004563808441, 0.33788633346557617, 0.3369083106517792, 0.33790579438209534, 0.3383057415485382, 0.33740365505218506, 0.33823373913764954, 0.33854320645332336, 0.33794277906417847, 0.3387961983680725, 0.3362913429737091, 0.3348880708217621, 0.3338857591152191, 0.3323822617530823, 0.33730632066726685, 0.33354708552360535, 0.3360753059387207, 0.33632346987724304, 0.3355313241481781, 0.33718857169151306, 0.33811694383621216, 0.33621934056282043, 0.3384585380554199, 0.33752918243408203, 0.3378259837627411, 0.3388069272041321, 0.33669424057006836, 0.33921658992767334, 0.3382152318954468, 0.3364450931549072, 0.33806926012039185, 0.33709418773651123, 0.3374279737472534, 0.337546706199646, 0.33614441752433777, 0.3394608497619629, 0.33540287613868713, 0.33839431405067444, 0.3376469314098358, 0.33604514598846436, 0.33435967564582825, 0.3354310989379883, 0.33627966046333313, 0.3372703194618225, 0.336254358291626, 0.33588653802871704, 0.33451634645462036, 0.3374289572238922, 0.3363040089607239, 0.3390764594078064, 0.33511286973953247, 0.33794471621513367, 0.3368908166885376, 0.3362436592578888, 0.33845949172973633, 0.33849552273750305, 0.33842933177948, 0.3395503759384155, 0.3372576832771301, 0.3389596939086914, 0.3380225598812103, 0.33915236592292786, 0.3380994498729706, 0.3373141288757324, 0.3386288285255432, 0.33915141224861145, 0.34040772914886475, 0.3378269672393799, 0.33709418773651123, 0.3381928503513336, 0.3390063941478729, 0.337232381105423, 0.3364733159542084, 0.3372362554073334, 0.3382571041584015, 0.33898890018463135, 0.33927303552627563, 0.3366796374320984, 0.3374503552913666, 0.3380361795425415, 0.33778706192970276, 0.33685383200645447, 0.3360733687877655, 0.33866482973098755, 0.33881664276123047, 0.33648985624313354, 0.3365677297115326, 0.3395134210586548, 0.3341553211212158, 0.33898597955703735, 0.33696088194847107, 0.33418840169906616, 0.33888769149780273, 0.3342331647872925, 0.33762454986572266, 0.33528122305870056, 0.3377783000469208, 0.3397148549556732, 0.33583593368530273, 0.3394637703895569, 0.3354729413986206, 0.3396739661693573, 0.3370065987110138, 0.3397946357727051, 0.3403824269771576, 0.33859962224960327, 0.3399941325187683, 0.3395766615867615, 0.33904337882995605, 0.3409108519554138, 0.33965158462524414, 0.33935868740081787, 0.33927011489868164, 0.3386794328689575, 0.33860352635383606, 0.33920785784721375, 0.3384721577167511, 0.3355741500854492, 0.3363857567310333, 0.33910176157951355, 0.3368372917175293, 0.34019267559051514]</t>
+  </si>
+  <si>
     <t>[0.12236528098583221, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568, 0.2850739061832428, 0.31206485629081726, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568, 0.3135908544063568]</t>
   </si>
   <si>
+    <t>[0.24444444477558136, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.27420124411582947, 0.27410587668418884, 0.299761563539505, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.31330472230911255, 0.3116833567619324, 0.31196948885917664, 0.31206485629081726, 0.31292322278022766, 0.3130185902118683, 0.31282785534858704, 0.3114926218986511, 0.3116833567619324, 0.30891749262809753, 0.3125417232513428, 0.3052932620048523, 0.3131139576435089, 0.30863139033317566, 0.30424416065216064, 0.3087267577648163, 0.3131139576435089, 0.3044348955154419, 0.30414879322052, 0.3095851242542267, 0.3096804916858673, 0.3083452582359314, 0.3101573586463928, 0.31025275588035583, 0.3065331280231476, 0.3070100247859955, 0.31063422560691833, 0.3104434907436371, 0.30720075964927673, 0.30891749262809753, 0.31034812331199646, 0.30739152431488037, 0.30739152431488037, 0.3092036247253418, 0.307486891746521, 0.3075822591781616, 0.30805912613868713, 0.3065331280231476, 0.3095851242542267, 0.3113018572330475, 0.3066285252571106, 0.30891749262809753, 0.3132093548774719, 0.3088221251964569, 0.31025275588035583, 0.3095851242542267, 0.30891749262809753, 0.3134954571723938, 0.30548402667045593, 0.3092036247253418, 0.3125417232513428, 0.30948975682258606, 0.31034812331199646, 0.30863139033317566, 0.3134000897407532, 0.30557939410209656, 0.30987125635147095, 0.3134000897407532, 0.31072962284088135, 0.30977585911750793, 0.30691462755203247, 0.3134000897407532, 0.31063422560691833, 0.30891749262809753, 0.31368622183799744, 0.3110157251358032, 0.31206485629081726, 0.308440625667572, 0.31282785534858704, 0.3122555911540985, 0.31072962284088135, 0.3109203577041626, 0.3131139576435089, 0.30433952808380127, 0.31282785534858704, 0.30119216442108154, 0.3095851242542267, 0.3126370906829834, 0.3035765290260315, 0.29737719893455505, 0.3056747615337372, 0.31244635581970215, 0.3135908544063568, 0.31063422560691833, 0.30901288986206055, 0.31292322278022766, 0.3126370906829834, 0.30805912613868713, 0.3067238926887512, 0.3109203577041626, 0.31292322278022766, 0.31063422560691833, 0.30596089363098145, 0.30720075964927673, 0.3125417232513428, 0.3134954571723938, 0.31111112236976624, 0.3079637587070465, 0.30948975682258606, 0.31063422560691833, 0.311778724193573, 0.3109203577041626, 0.3101573586463928, 0.3100619912147522, 0.310824990272522, 0.3132093548774719, 0.3134000897407532, 0.31120648980140686, 0.3110157251358032, 0.3116833567619324, 0.3109203577041626, 0.3104434907436371, 0.3109203577041626, 0.3113018572330475, 0.31292322278022766, 0.3122555911540985, 0.31072962284088135, 0.3118740916252136, 0.3121602237224579, 0.31034812331199646, 0.31158798933029175, 0.3116833567619324, 0.3140677213668823, 0.30910825729370117, 0.3140677213668823, 0.30948975682258606, 0.3139723539352417, 0.30643776059150696, 0.3113972246646881, 0.31378158926963806, 0.3114926218986511, 0.3140677213668823, 0.3105388581752777, 0.3134954571723938, 0.31111112236976624, 0.3092989921569824, 0.31378158926963806, 0.31034812331199646, 0.3135908544063568, 0.3130185902118683, 0.31196948885917664, 0.3134000897407532, 0.310824990272522, 0.3144492208957672, 0.30510252714157104, 0.31368622183799744, 0.3067238926887512, 0.3140677213668823, 0.31416308879852295, 0.3113018572330475, 0.31378158926963806, 0.3130185902118683, 0.31416308879852295, 0.3134954571723938, 0.31063422560691833, 0.31416308879852295, 0.3121602237224579, 0.3096804916858673, 0.31416308879852295, 0.31206485629081726, 0.31416308879852295, 0.310824990272522, 0.3121602237224579, 0.3156890869140625, 0.31292322278022766, 0.315116822719574, 0.3032904267311096, 0.3134954571723938, 0.3092036247253418, 0.30977585911750793, 0.3135908544063568, 0.3035765290260315, 0.3105388581752777, 0.3134000897407532, 0.30824989080429077, 0.31282785534858704, 0.3140677213668823, 0.3114926218986511, 0.31025275588035583, 0.31502145528793335, 0.31072962284088135, 0.31416308879852295, 0.3148307204246521, 0.3116833567619324, 0.3144492208957672, 0.31502145528793335, 0.3118740916252136, 0.3121602237224579, 0.3118740916252136, 0.31368622183799744, 0.31158798933029175, 0.3139723539352417, 0.31721505522727966, 0.31120648980140686, 0.3144492208957672, 0.3057701587677002, 0.31292322278022766, 0.29051026701927185, 0.30300429463386536, 0.31454458832740784, 0.315116822719574, 0.3149260878562927, 0.31463995575904846, 0.3113018572330475, 0.3118740916252136, 0.31502145528793335, 0.31454458832740784, 0.31158798933029175, 0.31378158926963806, 0.3134000897407532, 0.311778724193573, 0.3110157251358032, 0.3105388581752777, 0.3116833567619324, 0.3147353231906891, 0.3105388581752777, 0.3116833567619324, 0.3164520859718323, 0.31463995575904846, 0.3095851242542267, 0.3142584562301636, 0.3061516582965851, 0.3132093548774719, 0.2856461703777313, 0.30128756165504456, 0.31416308879852295, 0.31587982177734375, 0.3109203577041626, 0.31540295481681824, 0.3142584562301636, 0.3127324879169464, 0.3164520859718323, 0.31635668873786926, 0.315212219953537, 0.3131139576435089, 0.315212219953537, 0.3134000897407532, 0.30939435958862305, 0.31025275588035583, 0.3125417232513428, 0.31454458832740784, 0.3116833567619324, 0.3101573586463928, 0.3122555911540985, 0.31292322278022766, 0.31683358550071716, 0.3088221251964569, 0.315212219953537, 0.29566046595573425, 0.315116822719574, 0.31673818826675415, 0.30157366394996643, 0.3147353231906891, 0.31587982177734375, 0.3092036247253418, 0.3134000897407532, 0.31416308879852295, 0.311778724193573, 0.3143538534641266, 0.3155937194824219, 0.31282785534858704, 0.3134000897407532, 0.31673818826675415, 0.31673818826675415, 0.30987125635147095, 0.3122555911540985, 0.315212219953537, 0.3126370906829834, 0.3144492208957672, 0.3149260878562927, 0.3127324879169464, 0.31463995575904846, 0.3116833567619324, 0.3169289529323578, 0.31244635581970215, 0.3147353231906891, 0.3096804916858673, 0.31502145528793335, 0.29012876749038696, 0.3166428208351135, 0.3190271854400635, 0.3083452582359314, 0.3157844543457031, 0.31721505522727966, 0.3067238926887512, 0.31979018449783325, 0.3165474534034729, 0.3147353231906891, 0.32026705145835876, 0.31940868496894836, 0.31540295481681824, 0.3138769567012787, 0.3147353231906891, 0.3132093548774719, 0.3134000897407532, 0.3134000897407532, 0.3114926218986511, 0.31721505522727966, 0.3113972246646881, 0.3159751892089844, 0.30548402667045593, 0.3157844543457031, 0.29642346501350403, 0.31807345151901245, 0.3164520859718323, 0.30720075964927673, 0.31855031847953796, 0.3182641863822937, 0.31454458832740784, 0.319504052400589, 0.31454458832740784, 0.31454458832740784, 0.31883642077445984, 0.3114926218986511, 0.31769195199012756, 0.3139723539352417, 0.3164520859718323, 0.3173104524612427, 0.3116833567619324, 0.31540295481681824, 0.30777302384376526, 0.3195994198322296, 0.3005245625972748, 0.316165953874588, 0.3217930495738983, 0.31368622183799744, 0.3159751892089844, 0.3101573586463928, 0.3181688189506531, 0.31883642077445984, 0.31072962284088135, 0.3131139576435089, 0.31626132130622864, 0.31540295481681824, 0.3208392858505249, 0.30596089363098145, 0.316165953874588, 0.3166428208351135, 0.3114926218986511, 0.3183595538139343, 0.31025275588035583, 0.3067238926887512, 0.3203624188899994, 0.3118740916252136, 0.31282785534858704, 0.31292322278022766, 0.3142584562301636, 0.31683358550071716, 0.31206485629081726, 0.3092036247253418, 0.31673818826675415, 0.3160705864429474, 0.3135908544063568, 0.31378158926963806, 0.31416308879852295, 0.3177873194217682, 0.3134954571723938, 0.31759655475616455, 0.2925131022930145, 0.31330472230911255, 0.31120648980140686, 0.3028135299682617, 0.3166428208351135, 0.316165953874588, 0.2971864640712738, 0.3160705864429474, 0.3209346830844879, 0.3139723539352417, 0.31206485629081726, 0.3187410533428192, 0.32026705145835876, 0.3149260878562927, 0.3178826868534088, 0.32017168402671814, 0.3130185902118683, 0.315116822719574, 0.31626132130622864, 0.31330472230911255, 0.3142584562301636, 0.3173104524612427, 0.3116833567619324, 0.3157844543457031, 0.31454458832740784, 0.3121602237224579, 0.3191225528717041, 0.30634239315986633, 0.320553183555603, 0.315212219953537, 0.31759655475616455, 0.3182641863822937, 0.31111112236976624, 0.32150691747665405, 0.31540295481681824, 0.3156890869140625, 0.3159751892089844, 0.3121602237224579, 0.32026705145835876, 0.30987125635147095, 0.3216976523399353, 0.3135908544063568, 0.3118740916252136, 0.3203624188899994, 0.30977585911750793, 0.3190271854400635, 0.310824990272522, 0.31292322278022766, 0.3217930495738983, 0.30948975682258606, 0.32026705145835876, 0.31292322278022766, 0.3125417232513428, 0.31893181800842285, 0.2975679636001587, 0.31292322278022766, 0.3170243203639984, 0.3116833567619324, 0.3174058198928833, 0.31072962284088135, 0.30548402667045593, 0.3175011873245239, 0.3134000897407532, 0.3135908544063568, 0.3160705864429474, 0.3134000897407532, 0.3138769567012787, 0.31883642077445984, 0.31683358550071716, 0.31378158926963806, 0.3130185902118683, 0.3138769567012787, 0.3195994198322296, 0.3126370906829834, 0.31940868496894836, 0.3083452582359314, 0.3212207853794098, 0.3203624188899994, 0.3114926218986511, 0.31330472230911255, 0.299761563539505, 0.32064855098724365, 0.31721505522727966, 0.3175011873245239, 0.31969478726387024, 0.31120648980140686, 0.3200762867927551, 0.3164520859718323, 0.31463995575904846, 0.3191225528717041, 0.30815449357032776, 0.3182641863822937, 0.31759655475616455, 0.320553183555603, 0.3149260878562927, 0.31378158926963806, 0.3121602237224579, 0.32236528396606445, 0.3110157251358032, 0.3153075873851776, 0.2929899990558624, 0.3224606513977051, 0.3221745491027832, 0.315212219953537, 0.3175011873245239, 0.3132093548774719, 0.31120648980140686, 0.3181688189506531, 0.319504052400589, 0.311778724193573, 0.3130185902118683, 0.3190271854400635, 0.31673818826675415, 0.3160705864429474, 0.31196948885917664, 0.3148307204246521, 0.3181688189506531, 0.3116833567619324, 0.3160705864429474, 0.31120648980140686, 0.31883642077445984, 0.31206485629081726, 0.32064855098724365, 0.3061516582965851, 0.3178826868534088, 0.311778724193573, 0.31635668873786926, 0.3192179203033447, 0.30948975682258606, 0.3110157251358032, 0.3135908544063568, 0.31807345151901245, 0.3195994198322296, 0.3079637587070465, 0.31549832224845886, 0.31330472230911255, 0.3121602237224579, 0.3209346830844879, 0.2971864640712738, 0.31845492124557495, 0.3191225528717041, 0.3127324879169464, 0.31940868496894836, 0.30634239315986633, 0.30643776059150696, 0.3195994198322296, 0.3153075873851776, 0.3174058198928833, 0.3208392858505249, 0.3131139576435089, 0.3147353231906891, 0.31969478726387024, 0.3058655261993408, 0.3174058198928833, 0.31206485629081726, 0.3134000897407532, 0.3190271854400635, 0.31378158926963806, 0.31463995575904846, 0.31206485629081726, 0.311778724193573, 0.3214115500450134, 0.31120648980140686, 0.31206485629081726, 0.31683358550071716, 0.30977585911750793, 0.31969478726387024, 0.31292322278022766, 0.31034812331199646, 0.3199809193611145, 0.3156890869140625, 0.3173104524612427, 0.3118740916252136, 0.3123509883880615, 0.3192179203033447, 0.3144492208957672, 0.31673818826675415, 0.3065331280231476, 0.31940868496894836, 0.3164520859718323, 0.31711968779563904, 0.3100619912147522, 0.3178826868534088, 0.31330472230911255, 0.31769195199012756, 0.30729612708091736, 0.31807345151901245, 0.31378158926963806, 0.3178826868534088, 0.3105388581752777, 0.31330472230911255, 0.3138769567012787, 0.31635668873786926, 0.3087267577648163, 0.31454458832740784, 0.3116833567619324, 0.31626132130622864, 0.2923223674297333, 0.3139723539352417, 0.3174058198928833, 0.3058655261993408, 0.31769195199012756, 0.295469731092453, 0.30977585911750793, 0.3200762867927551, 0.3143538534641266, 0.3092036247253418, 0.31244635581970215, 0.311778724193573, 0.3100619912147522, 0.31711968779563904, 0.3140677213668823, 0.3113018572330475, 0.31292322278022766, 0.3160705864429474, 0.30977585911750793, 0.311778724193573, 0.3104434907436371, 0.31502145528793335, 0.3127324879169464, 0.3165474534034729, 0.31034812331199646, 0.316165953874588, 0.30729612708091736, 0.31855031847953796, 0.30853599309921265, 0.316165953874588, 0.31463995575904846, 0.3140677213668823, 0.3126370906829834, 0.31282785534858704, 0.3174058198928833, 0.3071053922176361, 0.3144492208957672, 0.29642346501350403, 0.3164520859718323, 0.3169289529323578]</t>
+  </si>
+  <si>
+    <t>[0.24444444477558136, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.27420124411582947, 0.27410587668418884, 0.299761563539505, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.31330472230911255, 0.3116833567619324, 0.31196948885917664, 0.31206485629081726, 0.31292322278022766, 0.3130185902118683, 0.31282785534858704, 0.3114926218986511, 0.3116833567619324, 0.30891749262809753, 0.3125417232513428, 0.3052932620048523, 0.3131139576435089, 0.30863139033317566, 0.30424416065216064, 0.3087267577648163, 0.3131139576435089, 0.3044348955154419, 0.30414879322052, 0.3095851242542267, 0.3096804916858673, 0.3083452582359314, 0.3101573586463928, 0.31025275588035583, 0.3065331280231476, 0.3070100247859955, 0.31063422560691833, 0.3104434907436371, 0.30720075964927673, 0.30891749262809753, 0.31034812331199646, 0.30739152431488037, 0.30739152431488037, 0.3092036247253418, 0.307486891746521, 0.3075822591781616, 0.30805912613868713, 0.3065331280231476, 0.3095851242542267, 0.3113018572330475, 0.3066285252571106, 0.30891749262809753, 0.3132093548774719, 0.3088221251964569, 0.31025275588035583, 0.3095851242542267, 0.30891749262809753, 0.3127324879169464, 0.27982833981513977, 0.2671435475349426, 0.25855985283851624, 0.25598475337028503, 0.2576060891151428, 0.2627563178539276, 0.27200764417648315, 0.3058655261993408, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.3130185902118683, 0.31330472230911255, 0.3121602237224579, 0.3110157251358032, 0.3104434907436371, 0.3092036247253418, 0.3088221251964569, 0.3088221251964569, 0.3087267577648163, 0.30824989080429077, 0.30815449357032776, 0.30824989080429077, 0.30824989080429077, 0.30863139033317566, 0.30891749262809753, 0.3087267577648163, 0.30901288986206055, 0.30805912613868713, 0.3078683912754059, 0.30767762660980225, 0.30767762660980225, 0.307486891746521, 0.3079637587070465, 0.30863139033317566, 0.30910825729370117, 0.3092036247253418, 0.3088221251964569, 0.308440625667572, 0.30815449357032776, 0.30901288986206055, 0.3099666237831116, 0.30910825729370117, 0.3096804916858673, 0.3096804916858673, 0.3096804916858673, 0.3100619912147522, 0.3095851242542267, 0.31120648980140686, 0.30863139033317566, 0.31158798933029175, 0.30901288986206055, 0.3116833567619324, 0.31111112236976624, 0.3114926218986511, 0.31158798933029175, 0.3113972246646881, 0.31034812331199646, 0.3113972246646881, 0.31111112236976624, 0.3109203577041626, 0.3134954571723938, 0.30433952808380127, 0.3125417232513428, 0.31292322278022766, 0.3058655261993408, 0.30863139033317566, 0.3130185902118683, 0.31330472230911255, 0.31034812331199646, 0.30681926012039185, 0.3088221251964569, 0.3118740916252136, 0.3130185902118683, 0.3121602237224579, 0.3122555911540985, 0.31158798933029175, 0.31206485629081726, 0.2333810180425644, 0.27887457609176636, 0.30605626106262207, 0.3127324879169464, 0.3123509883880615, 0.29995229840278625, 0.30128756165504456, 0.3058655261993408, 0.3006199300289154, 0.3013829290866852, 0.307486891746521, 0.3100619912147522, 0.3113972246646881, 0.3127324879169464, 0.3127324879169464, 0.3127324879169464, 0.311778724193573, 0.311778724193573, 0.3100619912147522, 0.30824989080429077, 0.3078683912754059, 0.30720075964927673, 0.30777302384376526, 0.307486891746521, 0.30853599309921265, 0.30910825729370117, 0.3101573586463928, 0.3101573586463928, 0.30977585911750793, 0.3087267577648163, 0.3075822591781616, 0.307486891746521, 0.3078683912754059, 0.30939435958862305, 0.31025275588035583, 0.3109203577041626, 0.31072962284088135, 0.3096804916858673, 0.3087267577648163, 0.30910825729370117, 0.30939435958862305, 0.30948975682258606, 0.3099666237831116, 0.30977585911750793, 0.3096804916858673, 0.3096804916858673, 0.3100619912147522, 0.3101573586463928, 0.3109203577041626, 0.3110157251358032, 0.3105388581752777, 0.31063422560691833, 0.31072962284088135, 0.3113018572330475, 0.3116833567619324, 0.3105388581752777, 0.31111112236976624, 0.3122555911540985, 0.31282785534858704, 0.31196948885917664, 0.3123509883880615, 0.3116833567619324, 0.31111112236976624, 0.31206485629081726, 0.3116833567619324, 0.311778724193573, 0.3118740916252136, 0.31111112236976624, 0.31206485629081726, 0.31025275588035583, 0.3127324879169464, 0.31111112236976624, 0.3096804916858673, 0.31206485629081726, 0.30910825729370117, 0.3123509883880615, 0.30948975682258606, 0.3099666237831116, 0.3122555911540985, 0.3079637587070465, 0.3122555911540985, 0.3087267577648163, 0.3123509883880615, 0.30977585911750793, 0.3104434907436371, 0.31368622183799744, 0.3092989921569824, 0.30853599309921265, 0.3131139576435089, 0.3104434907436371, 0.31063422560691833, 0.31282785534858704, 0.3123509883880615, 0.3088221251964569, 0.31034812331199646, 0.3113018572330475, 0.3114926218986511, 0.30948975682258606, 0.3110157251358032, 0.3135908544063568, 0.3092989921569824, 0.3092989921569824, 0.31292322278022766, 0.31282785534858704, 0.3088221251964569, 0.31111112236976624, 0.3116833567619324, 0.31282785534858704, 0.3101573586463928, 0.3101573586463928, 0.31416308879852295, 0.31206485629081726, 0.3105388581752777, 0.31244635581970215, 0.3125417232513428, 0.3121602237224579, 0.3113972246646881, 0.3134000897407532, 0.31378158926963806, 0.3134954571723938, 0.3122555911540985, 0.3140677213668823, 0.3142584562301636, 0.3116833567619324, 0.3134954571723938, 0.3140677213668823, 0.3053886592388153, 0.31368622183799744, 0.3134000897407532, 0.30519789457321167, 0.31368622183799744, 0.31368622183799744, 0.3135908544063568, 0.30987125635147095, 0.3100619912147522, 0.31330472230911255, 0.31196948885917664, 0.3114926218986511, 0.31416308879852295, 0.3118740916252136, 0.31244635581970215, 0.3149260878562927, 0.3143538534641266, 0.310824990272522, 0.31368622183799744, 0.31454458832740784, 0.3135908544063568, 0.3131139576435089, 0.31463995575904846, 0.3114926218986511, 0.315116822719574, 0.3134000897407532, 0.3156890869140625, 0.31454458832740784, 0.31282785534858704, 0.3142584562301636, 0.3159751892089844, 0.3036719262599945, 0.3135908544063568, 0.31368622183799744, 0.31502145528793335, 0.3149260878562927, 0.3127324879169464, 0.3140677213668823, 0.3144492208957672, 0.3105388581752777, 0.31587982177734375, 0.31416308879852295, 0.31502145528793335, 0.3153075873851776, 0.3126370906829834, 0.31378158926963806, 0.3156890869140625, 0.3164520859718323, 0.3155937194824219, 0.3126370906829834, 0.31635668873786926, 0.29260849952697754, 0.316165953874588, 0.3159751892089844, 0.3131139576435089, 0.315212219953537, 0.3142584562301636, 0.31292322278022766, 0.31635668873786926, 0.315212219953537, 0.31158798933029175, 0.3159751892089844, 0.3148307204246521, 0.31711968779563904, 0.31626132130622864, 0.31721505522727966, 0.31807345151901245, 0.31454458832740784, 0.3169289529323578, 0.2976633310317993, 0.3134954571723938, 0.3095851242542267, 0.3096804916858673, 0.3157844543457031, 0.3142584562301636, 0.3095851242542267, 0.3165474534034729, 0.3160705864429474, 0.3173104524612427, 0.31034812331199646, 0.3140677213668823, 0.3170243203639984, 0.311778724193573, 0.31549832224845886, 0.3166428208351135, 0.31721505522727966, 0.3155937194824219, 0.3192179203033447, 0.3175011873245239, 0.3178826868534088, 0.31845492124557495, 0.31206485629081726, 0.3181688189506531, 0.310824990272522, 0.31683358550071716, 0.307486891746521, 0.31769195199012756, 0.3125417232513428, 0.3165474534034729, 0.3166428208351135, 0.310824990272522, 0.3183595538139343, 0.30987125635147095, 0.3178826868534088, 0.3166428208351135, 0.3144492208957672, 0.31797805428504944, 0.3088221251964569, 0.31769195199012756, 0.31292322278022766, 0.3155937194824219, 0.3182641863822937, 0.3109203577041626, 0.3166428208351135, 0.307486891746521, 0.31797805428504944, 0.32026705145835876, 0.31158798933029175, 0.3175011873245239, 0.3113018572330475, 0.3190271854400635, 0.3186456859111786, 0.31034812331199646, 0.3166428208351135, 0.3109203577041626, 0.3153075873851776, 0.31845492124557495, 0.3100619912147522, 0.3199809193611145, 0.31244635581970215, 0.31893181800842285, 0.31683358550071716, 0.3122555911540985, 0.3181688189506531, 0.3113972246646881, 0.3178826868534088, 0.31158798933029175, 0.31769195199012756, 0.3127324879169464, 0.3170243203639984, 0.3187410533428192, 0.3149260878562927, 0.3174058198928833, 0.3130185902118683, 0.31721505522727966, 0.2856461703777313, 0.31158798933029175, 0.3186456859111786, 0.2979494631290436, 0.3186456859111786, 0.3160705864429474, 0.3199809193611145, 0.3088221251964569, 0.3190271854400635, 0.31587982177734375, 0.3149260878562927, 0.31158798933029175, 0.3191225528717041, 0.31683358550071716, 0.3182641863822937, 0.3166428208351135, 0.3195994198322296, 0.31711968779563904, 0.3135908544063568, 0.3159751892089844, 0.31244635581970215, 0.3147353231906891, 0.3153075873851776, 0.3156890869140625, 0.31711968779563904, 0.31454458832740784, 0.3186456859111786, 0.3127324879169464, 0.31711968779563904, 0.2989031970500946, 0.32045778632164, 0.31797805428504944, 0.30634239315986633, 0.31883642077445984, 0.320553183555603, 0.30824989080429077, 0.3198855519294739, 0.3198855519294739, 0.3153075873851776, 0.31883642077445984, 0.3182641863822937, 0.3147353231906891, 0.3199809193611145, 0.3165474534034729, 0.3142584562301636, 0.3186456859111786, 0.3159751892089844, 0.31893181800842285, 0.3147353231906891, 0.3199809193611145, 0.31635668873786926, 0.31845492124557495, 0.3155937194824219, 0.3187410533428192, 0.31721505522727966, 0.3173104524612427, 0.3155937194824219, 0.3190271854400635, 0.2957558333873749, 0.31683358550071716, 0.31855031847953796, 0.31206485629081726, 0.31807345151901245, 0.3209346830844879, 0.3083452582359314, 0.3191225528717041, 0.31855031847953796, 0.3127324879169464, 0.3207439184188843, 0.32103005051612854, 0.31883642077445984, 0.3191225528717041, 0.32026705145835876, 0.31711968779563904, 0.3165474534034729, 0.3149260878562927, 0.3191225528717041, 0.3164520859718323, 0.31855031847953796, 0.3181688189506531, 0.3187410533428192, 0.3122555911540985, 0.3190271854400635, 0.2929899990558624, 0.3198855519294739, 0.3169289529323578, 0.31034812331199646, 0.31855031847953796, 0.3200762867927551, 0.3113018572330475, 0.31711968779563904, 0.3191225528717041, 0.31540295481681824, 0.3203624188899994, 0.320553183555603, 0.31463995575904846, 0.31845492124557495, 0.3183595538139343, 0.316165953874588, 0.31940868496894836, 0.3159751892089844, 0.3169289529323578, 0.3200762867927551, 0.3175011873245239, 0.31883642077445984, 0.3178826868534088, 0.3195994198322296, 0.3144492208957672, 0.31979018449783325, 0.3142584562301636]</t>
+  </si>
+  <si>
+    <t>[0.2654268145561218, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.30519789457321167, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.30739152431488037, 0.3053886592388153, 0.3053886592388153, 0.30824989080429077, 0.3053886592388153, 0.30729612708091736, 0.3053886592388153, 0.30557939410209656, 0.30557939410209656, 0.30739152431488037, 0.3062470257282257, 0.3053886592388153, 0.30729612708091736, 0.3058655261993408, 0.3044348955154419, 0.3052932620048523, 0.30414879322052, 0.30596089363098145, 0.3056747615337372, 0.30596089363098145, 0.3053886592388153, 0.3053886592388153, 0.304053395986557, 0.30472102761268616, 0.3053886592388153, 0.30691462755203247, 0.3058655261993408, 0.30605626106262207, 0.3053886592388153, 0.3071053922176361, 0.3062470257282257, 0.3053886592388153, 0.3070100247859955, 0.30605626106262207, 0.3058655261993408, 0.30634239315986633, 0.30634239315986633, 0.30767762660980225, 0.3052932620048523, 0.3067238926887512, 0.30691462755203247, 0.30519789457321167, 0.3071053922176361, 0.3066285252571106, 0.30634239315986633, 0.30729612708091736, 0.30720075964927673, 0.30739152431488037, 0.30548402667045593, 0.30777302384376526, 0.3078683912754059, 0.30777302384376526, 0.3078683912754059, 0.30729612708091736, 0.30634239315986633, 0.30433952808380127, 0.3083452582359314, 0.30910825729370117, 0.3092989921569824, 0.307486891746521, 0.3061516582965851, 0.3083452582359314, 0.30891749262809753, 0.3079637587070465, 0.3092036247253418, 0.3079637587070465, 0.307486891746521, 0.3049117922782898, 0.3067238926887512, 0.3022412955760956, 0.30777302384376526, 0.30729612708091736, 0.3049117922782898, 0.30948975682258606, 0.30691462755203247, 0.30605626106262207, 0.30729612708091736, 0.30739152431488037, 0.3071053922176361, 0.2794468402862549, 0.2730567455291748, 0.2929899990558624, 0.3036719262599945, 0.28612303733825684, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3053886592388153, 0.3057701587677002, 0.30634239315986633, 0.3065331280231476, 0.30681926012039185, 0.30691462755203247, 0.30729612708091736, 0.30824989080429077, 0.30891749262809753, 0.3088221251964569, 0.3087267577648163, 0.30824989080429077, 0.30891749262809753, 0.3092036247253418, 0.30987125635147095, 0.3101573586463928, 0.30977585911750793, 0.31034812331199646, 0.3104434907436371, 0.3104434907436371, 0.31034812331199646, 0.31025275588035583, 0.3104434907436371, 0.30891749262809753, 0.3088221251964569, 0.3096804916858673, 0.31120648980140686, 0.3099666237831116, 0.30987125635147095, 0.30901288986206055, 0.3092989921569824, 0.3101573586463928, 0.31034812331199646, 0.31063422560691833, 0.31034812331199646, 0.30910825729370117, 0.308440625667572, 0.30720075964927673, 0.30910825729370117, 0.3083452582359314, 0.31158798933029175, 0.310824990272522, 0.3092036247253418, 0.3088221251964569, 0.3083452582359314, 0.3096804916858673, 0.3092036247253418, 0.311778724193573, 0.31206485629081726, 0.31072962284088135, 0.3099666237831116, 0.30939435958862305, 0.308440625667572, 0.3121602237224579, 0.3126370906829834, 0.3122555911540985, 0.3138769567012787, 0.3105388581752777, 0.3130185902118683, 0.3126370906829834, 0.31120648980140686, 0.3126370906829834, 0.3116833567619324, 0.3140677213668823, 0.3131139576435089, 0.31196948885917664, 0.3142584562301636, 0.3122555911540985, 0.31587982177734375, 0.3142584562301636, 0.3156890869140625, 0.3166428208351135, 0.3122555911540985, 0.3121602237224579, 0.3109203577041626, 0.31587982177734375, 0.31587982177734375, 0.3160705864429474, 0.3134000897407532, 0.3144492208957672, 0.31540295481681824, 0.3166428208351135, 0.31463995575904846, 0.3138769567012787, 0.3143538534641266, 0.3192179203033447, 0.3110157251358032, 0.3182641863822937, 0.31855031847953796, 0.3142584562301636, 0.3186456859111786, 0.3183595538139343, 0.31635668873786926, 0.3170243203639984, 0.31940868496894836, 0.31711968779563904, 0.31683358550071716, 0.32045778632164, 0.3178826868534088, 0.30977585911750793, 0.30815449357032776, 0.3105388581752777, 0.31292322278022766, 0.3110157251358032, 0.31893181800842285, 0.3078683912754059, 0.3190271854400635, 0.31072962284088135, 0.31463995575904846, 0.31502145528793335, 0.31721505522727966, 0.3149260878562927, 0.3177873194217682, 0.31626132130622864, 0.3159751892089844, 0.31416308879852295, 0.3173104524612427, 0.3156890869140625, 0.3165474534034729, 0.31979018449783325, 0.31931331753730774, 0.31855031847953796, 0.31931331753730774, 0.32198378443717957, 0.31883642077445984, 0.31845492124557495, 0.31931331753730774, 0.32026705145835876, 0.31940868496894836, 0.31969478726387024, 0.3190271854400635, 0.31721505522727966, 0.32103005051612854, 0.3207439184188843, 0.3169289529323578, 0.3200762867927551, 0.31626132130622864, 0.31502145528793335, 0.3153075873851776, 0.32103005051612854, 0.3131139576435089, 0.3139723539352417, 0.31807345151901245, 0.3159751892089844, 0.31635668873786926, 0.31931331753730774, 0.3166428208351135, 0.3174058198928833, 0.3149260878562927, 0.319504052400589, 0.31883642077445984, 0.3199809193611145, 0.3198855519294739, 0.3199809193611145, 0.32045778632164, 0.32045778632164, 0.31969478726387024, 0.32064855098724365, 0.3199809193611145, 0.3200762867927551, 0.3203624188899994, 0.32017168402671814, 0.320553183555603, 0.320553183555603, 0.3216976523399353, 0.31979018449783325, 0.3157844543457031, 0.31540295481681824, 0.3186456859111786, 0.3217930495738983, 0.3170243203639984, 0.3170243203639984, 0.3203624188899994, 0.3177873194217682, 0.31759655475616455, 0.3217930495738983, 0.3203624188899994, 0.3220791518688202, 0.3200762867927551, 0.32026705145835876, 0.3225560188293457, 0.32112541794776917, 0.32188841700553894, 0.3209346830844879, 0.3221745491027832, 0.32045778632164, 0.3221745491027832, 0.3216022849082947, 0.3207439184188843, 0.3213161528110504, 0.32112541794776917, 0.32150691747665405, 0.3213161528110504, 0.32188841700553894, 0.3216976523399353, 0.3224606513977051, 0.3229375183582306, 0.32274678349494934, 0.3170243203639984, 0.3010967969894409, 0.3148307204246521, 0.3209346830844879, 0.31244635581970215, 0.315116822719574, 0.3144492208957672, 0.3203624188899994, 0.31979018449783325, 0.315212219953537, 0.3169289529323578, 0.3207439184188843, 0.31979018449783325, 0.31673818826675415, 0.3195994198322296, 0.3198855519294739, 0.3208392858505249, 0.31769195199012756, 0.32236528396606445, 0.320553183555603, 0.32017168402671814, 0.3214115500450134, 0.3217930495738983, 0.32150691747665405, 0.32112541794776917, 0.3230329155921936, 0.3213161528110504, 0.32103005051612854, 0.3216976523399353, 0.3226514160633087, 0.32198378443717957, 0.3217930495738983, 0.32236528396606445, 0.32198378443717957, 0.32112541794776917, 0.3220791518688202, 0.32274678349494934, 0.3216976523399353, 0.32198378443717957, 0.3220791518688202, 0.3217930495738983, 0.323795884847641, 0.3220791518688202, 0.32484501600265503, 0.32198378443717957, 0.3225560188293457, 0.3220791518688202, 0.3226514160633087, 0.32284215092658997, 0.3229375183582306, 0.3220791518688202, 0.3225560188293457, 0.3229375183582306, 0.32370051741600037, 0.323795884847641, 0.32150691747665405, 0.32226991653442383, 0.3208392858505249, 0.3221745491027832, 0.32274678349494934, 0.3217930495738983, 0.3224606513977051, 0.32322365045547485, 0.3233190178871155, 0.3224606513977051, 0.3229375183582306, 0.3225560188293457, 0.32370051741600037, 0.3225560188293457, 0.323795884847641, 0.323795884847641, 0.32274678349494934, 0.32398664951324463, 0.32322365045547485, 0.323795884847641, 0.32312828302383423, 0.32198378443717957, 0.3216022849082947, 0.32226991653442383, 0.32274678349494934, 0.3233190178871155, 0.3230329155921936, 0.3224606513977051, 0.32284215092658997, 0.3226514160633087, 0.3192179203033447, 0.31883642077445984, 0.3213161528110504, 0.3255126476287842, 0.32112541794776917, 0.32370051741600037, 0.3229375183582306, 0.3214115500450134, 0.3241773843765259, 0.3241773843765259, 0.32188841700553894, 0.3234144151210785, 0.3225560188293457, 0.32236528396606445, 0.3241773843765259, 0.32236528396606445, 0.3226514160633087, 0.3247496485710144, 0.3225560188293457, 0.323795884847641, 0.32312828302383423, 0.32360514998435974, 0.32494038343429565, 0.3230329155921936, 0.3233190178871155, 0.3229375183582306, 0.3213161528110504, 0.3212207853794098, 0.3225560188293457, 0.3220791518688202, 0.3246542811393738, 0.323891282081604, 0.3235097825527191, 0.32494038343429565, 0.3241773843765259, 0.3234144151210785, 0.3235097825527191, 0.3230329155921936, 0.3242727816104889, 0.32284215092658997, 0.3235097825527191, 0.3246542811393738, 0.32360514998435974, 0.32284215092658997, 0.32284215092658997, 0.3225560188293457, 0.32150691747665405, 0.32532188296318054, 0.32455888390541077, 0.32226991653442383, 0.3212207853794098, 0.3246542811393738, 0.32274678349494934, 0.323891282081604, 0.3252265155315399, 0.32312828302383423, 0.32312828302383423, 0.32484501600265503, 0.32541725039482117, 0.3246542811393738, 0.3233190178871155, 0.32446351647377014, 0.323891282081604, 0.323795884847641, 0.3241773843765259, 0.3250357508659363, 0.32484501600265503, 0.32541725039482117, 0.3246542811393738, 0.32532188296318054, 0.32589414715766907, 0.32322365045547485, 0.3247496485710144, 0.3241773843765259, 0.3252265155315399, 0.3251311480998993, 0.32494038343429565, 0.32532188296318054, 0.32656174898147583, 0.32541725039482117, 0.32455888390541077, 0.32360514998435974, 0.32455888390541077, 0.3241773843765259, 0.3234144151210785, 0.3252265155315399, 0.32408201694488525, 0.32618024945259094, 0.3256080150604248, 0.32446351647377014, 0.32398664951324463, 0.32446351647377014, 0.32398664951324463, 0.32494038343429565, 0.3278016149997711, 0.3247496485710144, 0.3255126476287842, 0.32455888390541077, 0.3260848820209503, 0.3264663815498352, 0.3247496485710144, 0.3259895145893097, 0.3264663815498352, 0.3259895145893097, 0.32618024945259094, 0.32618024945259094, 0.3250357508659363, 0.32761088013648987, 0.3259895145893097, 0.3226514160633087, 0.3225560188293457, 0.32675251364707947, 0.32532188296318054, 0.3224606513977051, 0.3264663815498352, 0.32494038343429565, 0.32236528396606445, 0.32484501600265503, 0.3264663815498352, 0.3243681490421295, 0.3246542811393738, 0.32570338249206543, 0.32398664951324463, 0.3260848820209503, 0.3246542811393738, 0.3259895145893097, 0.32665711641311646, 0.32627564668655396, 0.32589414715766907, 0.327229380607605, 0.32570338249206543, 0.32742011547088623, 0.3269432485103607, 0.3273247480392456, 0.32703861594200134, 0.3250357508659363, 0.3273247480392456, 0.32799237966537476, 0.3263710141181946, 0.32875537872314453, 0.32627564668655396, 0.3264663815498352, 0.32570338249206543, 0.3264663815498352, 0.32875537872314453, 0.32675251364707947, 0.3264663815498352, 0.3252265155315399, 0.32827848196029663, 0.32532188296318054, 0.32627564668655396, 0.3273247480392456, 0.3273247480392456, 0.3285646140575409, 0.32713401317596436, 0.32751551270484924, 0.3299952447414398, 0.32846924662590027, 0.32761088013648987, 0.3260848820209503, 0.32570338249206543, 0.32618024945259094, 0.32751551270484924, 0.32627564668655396, 0.32885074615478516, 0.32656174898147583, 0.32913684844970703, 0.32923224568367004, 0.32742011547088623, 0.32846924662590027, 0.3277062475681305, 0.3273247480392456, 0.32751551270484924, 0.32875537872314453, 0.3302813470363617, 0.3269432485103607, 0.32827848196029663, 0.32713401317596436, 0.3285646140575409, 0.3264663815498352, 0.32789698243141174, 0.32618024945259094, 0.32875537872314453, 0.3290414810180664, 0.32875537872314453, 0.32970911264419556, 0.32827848196029663, 0.32579874992370605, 0.32665711641311646, 0.3285646140575409, 0.3286599814891815, 0.32761088013648987, 0.3295183479785919, 0.32970911264419556, 0.32961374521255493, 0.32846924662590027, 0.3273247480392456, 0.327229380607605, 0.32970911264419556, 0.32970911264419556, 0.32885074615478516, 0.3316165804862976, 0.328183114528656, 0.328183114528656, 0.32913684844970703, 0.33056747913360596, 0.33056747913360596, 0.32875537872314453, 0.3311397135257721, 0.33009061217308044, 0.32913684844970703, 0.32713401317596436, 0.32799237966537476, 0.3285646140575409, 0.33018597960472107, 0.3298044800758362, 0.3294229805469513, 0.3294229805469513, 0.32932761311531067, 0.33142584562301636, 0.3280877470970154, 0.3295183479785919, 0.33104434609413147, 0.33142584562301636, 0.33056747913360596, 0.32846924662590027, 0.33104434609413147, 0.33180734515190125, 0.33009061217308044, 0.32675251364707947, 0.32799237966537476, 0.3298998475074768, 0.331521213054657, 0.32799237966537476, 0.33218884468078613, 0.3289461135864258, 0.33047211170196533, 0.3316165804862976, 0.3298998475074768, 0.3286599814891815, 0.33094897866249084, 0.33314257860183716, 0.32970911264419556, 0.32913684844970703, 0.33142584562301636, 0.3311397135257721, 0.3306628465652466, 0.33009061217308044, 0.3328564763069153, 0.3323795795440674, 0.3303767144680023, 0.33218884468078613, 0.33228421211242676, 0.3303767144680023, 0.3311397135257721, 0.3294229805469513, 0.3250357508659363, 0.33047211170196533, 0.32742011547088623, 0.32799237966537476, 0.32675251364707947, 0.32656174898147583, 0.3311397135257721, 0.32885074615478516, 0.3298998475074768, 0.32846924662590027, 0.3306628465652466, 0.32675251364707947, 0.32789698243141174, 0.3299952447414398, 0.3312351107597351, 0.33056747913360596, 0.3311397135257721, 0.32970911264419556, 0.3290414810180664, 0.3298998475074768, 0.33133047819137573, 0.33304721117019653, 0.33390557765960693, 0.33400094509124756, 0.3333333432674408, 0.3342870771884918, 0.33276107907295227, 0.33266571164131165, 0.331521213054657, 0.33352407813072205, 0.3328564763069153, 0.33352407813072205, 0.3341917097568512, 0.33304721117019653, 0.33314257860183716, 0.32913684844970703, 0.320553183555603, 0.3303767144680023, 0.32322365045547485, 0.32703861594200134, 0.3307582139968872, 0.32274678349494934, 0.32970911264419556, 0.3273247480392456, 0.3311397135257721, 0.3298044800758362, 0.33314257860183716, 0.332570344209671, 0.3317119777202606, 0.3312351107597351, 0.3312351107597351, 0.33142584562301636, 0.3338102102279663, 0.3323795795440674, 0.3307582139968872, 0.3323795795440674, 0.3323795795440674, 0.33314257860183716, 0.33266571164131165, 0.33218884468078613, 0.33400094509124756, 0.3355269432067871, 0.33390557765960693, 0.33485931158065796, 0.33361944556236267, 0.33361944556236267, 0.3319980800151825, 0.33047211170196533, 0.3299952447414398, 0.33266571164131165, 0.3324749767780304, 0.3319980800151825, 0.332570344209671, 0.33009061217308044, 0.33447781205177307, 0.3341917097568512, 0.33266571164131165, 0.33447781205177307, 0.33228421211242676, 0.3338102102279663, 0.33361944556236267, 0.33495470881462097, 0.33609917759895325, 0.3350500762462616, 0.33524081110954285, 0.33619457483291626, 0.33695754408836365, 0.336862176656723, 0.3380066752433777, 0.33609917759895325, 0.3354315757751465, 0.335908442735672, 0.3355269432067871, 0.33142584562301636, 0.3182641863822937, 0.3285646140575409, 0.32618024945259094, 0.3285646140575409, 0.32961374521255493, 0.3241773843765259, 0.3308536112308502, 0.32875537872314453, 0.33180734515190125, 0.332570344209671, 0.3308536112308502, 0.3319980800151825, 0.33266571164131165, 0.33133047819137573, 0.3333333432674408, 0.336862176656723, 0.332570344209671, 0.3355269432067871, 0.33476394414901733, 0.33190271258354187, 0.3328564763069153, 0.33361944556236267, 0.33447781205177307, 0.33447781205177307, 0.335908442735672, 0.33390557765960693, 0.33409634232521057, 0.3328564763069153, 0.33361944556236267, 0.3323795795440674, 0.33495470881462097, 0.33657607436180115, 0.3338102102279663, 0.33533620834350586, 0.33361944556236267, 0.3332379460334778, 0.331521213054657, 0.33447781205177307, 0.33476394414901733, 0.33562231063842773, 0.33562231063842773, 0.33438244462013245, 0.33533620834350586, 0.33495470881462097, 0.3363853096961975, 0.33476394414901733, 0.3367668092250824, 0.3377205431461334, 0.3375298082828522, 0.33562231063842773, 0.3363853096961975, 0.3338102102279663, 0.332570344209671, 0.33447781205177307, 0.3354315757751465, 0.3345732092857361, 0.33571767807006836, 0.3324749767780304, 0.3362899422645569, 0.33581307530403137, 0.33609917759895325, 0.3377205431461334, 0.33533620834350586, 0.3351454436779022, 0.3346685767173767, 0.3342870771884918, 0.3375298082828522, 0.33581307530403137, 0.33533620834350586, 0.3350500762462616, 0.33619457483291626, 0.3354315757751465, 0.33743444085121155, 0.33819741010665894, 0.3366714417934418, 0.33571767807006836, 0.33571767807006836, 0.3355269432067871, 0.33495470881462097, 0.3341917097568512, 0.33533620834350586, 0.33829280734062195, 0.33562231063842773, 0.3360038101673126, 0.3375298082828522, 0.33571767807006836, 0.3366714417934418, 0.33409634232521057, 0.33190271258354187, 0.33533620834350586, 0.33648067712783813, 0.33447781205177307, 0.3350500762462616, 0.3360038101673126, 0.33562231063842773, 0.33781594038009644, 0.3350500762462616, 0.3334287106990814, 0.33495470881462097, 0.3342870771884918, 0.3337148427963257, 0.33485931158065796, 0.3308536112308502, 0.336862176656723, 0.3307582139968872, 0.3323795795440674, 0.3328564763069153, 0.3354315757751465, 0.33495470881462097, 0.33571767807006836, 0.33524081110954285, 0.3354315757751465, 0.3360038101673126, 0.33791130781173706, 0.3380066752433777, 0.33619457483291626, 0.336862176656723, 0.33648067712783813, 0.3385789096355438, 0.33400094509124756, 0.33581307530403137, 0.33743444085121155, 0.3377205431461334, 0.3376251757144928, 0.33533620834350586, 0.3383881747722626, 0.34000954031944275, 0.3376251757144928, 0.33495470881462097, 0.3363853096961975, 0.33791130781173706, 0.3367668092250824, 0.3363853096961975, 0.3389604091644287, 0.3398187756538391, 0.3390558063983917, 0.3394373059272766, 0.336862176656723, 0.3360038101673126, 0.3341917097568512, 0.3351454436779022, 0.33609917759895325, 0.3342870771884918, 0.3355269432067871, 0.3372436761856079, 0.33619457483291626, 0.33571767807006836, 0.33438244462013245, 0.33695754408836365, 0.3354315757751465, 0.3394373059272766, 0.3377205431461334, 0.33648067712783813, 0.3351454436779022, 0.340295672416687, 0.3389604091644287, 0.33476394414901733, 0.34000954031944275, 0.3401049077510834, 0.33819741010665894, 0.33953267335891724, 0.33781594038009644, 0.33743444085121155, 0.3372436761856079, 0.3388650417327881, 0.3375298082828522, 0.3389604091644287, 0.33962804079055786, 0.33524081110954285, 0.3371483087539673, 0.33609917759895325, 0.3354315757751465, 0.3338102102279663, 0.3324749767780304, 0.34048640727996826, 0.33819741010665894, 0.3334287106990814, 0.3372436761856079, 0.33609917759895325, 0.3375298082828522, 0.3355269432067871, 0.33609917759895325, 0.33791130781173706, 0.3398187756538391, 0.33819741010665894, 0.336862176656723, 0.3409632742404938, 0.340295672416687, 0.3388650417327881, 0.33791130781173706, 0.33829280734062195, 0.34134477376937866, 0.3384835422039032, 0.3406771719455719, 0.3401049077510834, 0.33876967430114746, 0.3388650417327881, 0.33953267335891724, 0.3380066752433777, 0.3338102102279663, 0.33056747913360596, 0.32799237966537476, 0.3355269432067871, 0.3320934772491455, 0.33791130781173706, 0.33953267335891724, 0.33409634232521057, 0.33867430686950684, 0.3409632742404938, 0.3338102102279663, 0.3372436761856079, 0.3416309058666229, 0.3407725393772125, 0.33657607436180115, 0.3389604091644287, 0.343633770942688, 0.3393419086933136, 0.33791130781173706, 0.3405817747116089, 0.3407725393772125, 0.33867430686950684, 0.340200275182724, 0.34172627329826355, 0.33962804079055786, 0.33962804079055786, 0.33829280734062195, 0.33733904361724854, 0.3338102102279663, 0.3328564763069153, 0.33876967430114746, 0.3317119777202606, 0.3398187756538391, 0.3397234082221985, 0.3362899422645569, 0.3405817747116089, 0.34000954031944275, 0.33581307530403137, 0.34124940633773804, 0.3427754044532776, 0.3375298082828522, 0.3389604091644287, 0.34220314025878906, 0.3406771719455719, 0.3381020426750183, 0.33953267335891724, 0.34048640727996826, 0.33819741010665894, 0.3405817747116089, 0.34220314025878906, 0.33781594038009644, 0.3409632742404938, 0.3366714417934418, 0.3398187756538391, 0.3381020426750183, 0.3394373059272766, 0.3332379460334778, 0.33619457483291626, 0.3406771719455719, 0.3397234082221985, 0.33609917759895325, 0.3360038101673126, 0.33609917759895325, 0.33915117383003235, 0.3351454436779022, 0.34134477376937866, 0.3410586416721344, 0.3394373059272766, 0.3375298082828522, 0.3355269432067871, 0.34172627329826355, 0.34172627329826355, 0.3389604091644287, 0.3420124053955078, 0.3401049077510834, 0.3410586416721344, 0.3383881747722626, 0.3398187756538391, 0.3388650417327881, 0.33876967430114746, 0.33791130781173706, 0.3410586416721344, 0.3427754044532776, 0.33876967430114746, 0.33867430686950684, 0.33953267335891724, 0.340295672416687, 0.33819741010665894, 0.3376251757144928, 0.3393419086933136, 0.34220314025878906, 0.3418216407299042, 0.3398187756538391, 0.3346685767173767, 0.3416309058666229, 0.3393419086933136, 0.3376251757144928, 0.3376251757144928, 0.335908442735672, 0.3393419086933136, 0.3420124053955078, 0.33648067712783813, 0.339246541261673, 0.3407725393772125, 0.3362899422645569, 0.3422985076904297, 0.33791130781173706, 0.33829280734062195, 0.33876967430114746, 0.33619457483291626, 0.3367668092250824, 0.3380066752433777, 0.3377205431461334, 0.34172627329826355, 0.3363853096961975, 0.3406771719455719, 0.3381020426750183, 0.3415355384349823, 0.3376251757144928, 0.3398187756538391, 0.3422985076904297, 0.3397234082221985, 0.3415355384349823, 0.3418216407299042, 0.3427754044532776, 0.34220314025878906, 0.34086790680885315, 0.3419170379638672, 0.3426800072193146, 0.3397234082221985, 0.3384835422039032, 0.34048640727996826, 0.34124940633773804, 0.3360038101673126, 0.3397234082221985, 0.34172627329826355, 0.33619457483291626, 0.3407725393772125]</t>
+  </si>
+  <si>
     <t>[3.5162222385406494, 3.462643623352051, 3.3653926849365234, 3.206531286239624, 3.012010097503662, 2.9896275997161865, 2.899851083755493, 2.7783854007720947, 2.7431881427764893, 2.7289252281188965, 2.6971659660339355, 2.6490063667297363, 2.598536252975464, 2.5671865940093994, 2.5484681129455566, 2.527329921722412, 2.5052490234375, 2.4902026653289795]</t>
+  </si>
+  <si>
+    <t>[3.5095903873443604, 3.4489684104919434, 3.339707374572754, 3.162562608718872, 2.9825661182403564, 2.949648380279541, 2.8513505458831787, 2.786360263824463, 2.7651185989379883, 2.724621534347534, 2.6648411750793457, 2.605236291885376, 2.5667612552642822, 2.540367364883423, 2.4989113807678223, 2.4643256664276123, 2.4446396827697754, 2.4271960258483887, 2.408658266067505, 2.3920631408691406, 2.379755973815918, 2.36987042427063, 2.361659288406372, 2.3571841716766357, 2.3522145748138428, 2.3459131717681885, 2.342430353164673, 2.3393330574035645, 2.333306074142456, 2.328042984008789, 2.3236935138702393, 2.318352222442627, 2.3131792545318604, 2.3095407485961914, 2.305798053741455, 2.302851676940918, 2.3008761405944824, 2.297832489013672, 2.2941598892211914, 2.2913074493408203, 2.2881228923797607, 2.2848634719848633, 2.282146692276001, 2.279233932495117, 2.2768354415893555, 2.274467706680298, 2.2722373008728027, 2.2702736854553223, 2.268216133117676, 2.2661170959472656, 2.2639448642730713, 2.262059450149536, 2.2601139545440674, 2.258042097091675, 2.2562196254730225, 2.2544631958007812, 2.2526614665985107, 2.251073122024536, 2.2497000694274902, 2.2485225200653076, 2.249143362045288, 2.2541801929473877, 2.247641086578369, 2.245849847793579, 2.249382257461548, 2.2423505783081055, 2.2471234798431396, 2.243851661682129, 2.242658853530884, 2.243673086166382, 2.2394087314605713, 2.24165940284729, 2.2374486923217773, 2.2398855686187744, 2.2369229793548584, 2.2368404865264893, 2.236116647720337, 2.234091281890869, 2.235264778137207, 2.2325942516326904, 2.233319044113159, 2.2322986125946045, 2.2310378551483154, 2.2314419746398926, 2.231264591217041, 2.229811191558838, 2.229473829269409, 2.229574680328369, 2.227278232574463, 2.227938413619995, 2.227445363998413, 2.2258434295654297, 2.2254252433776855, 2.2259626388549805, 2.223963975906372, 2.223522901535034, 2.2240068912506104, 2.223832130432129, 2.2224514484405518, 2.2213029861450195, 2.2206268310546875, 2.2199296951293945, 2.2204864025115967, 2.220642328262329, 2.221252918243408, 2.221362352371216, 2.218933343887329, 2.2186779975891113, 2.2173237800598145, 2.218945264816284, 2.2181639671325684, 2.2176201343536377, 2.2147598266601562, 2.215036153793335, 2.213874101638794, 2.214340925216675, 2.213022232055664, 2.212801456451416, 2.2117385864257812, 2.211242914199829, 2.210810422897339, 2.2103545665740967, 2.2113752365112305, 2.2183918952941895, 2.2308545112609863, 2.251431941986084, 2.2215754985809326, 2.2493557929992676, 2.216662883758545, 2.2366116046905518, 2.2205448150634766, 2.2226762771606445, 2.2203729152679443, 2.2237436771392822, 2.2184267044067383, 2.214290142059326, 2.2216286659240723, 2.2123348712921143, 2.2167470455169678, 2.21290922164917, 2.2151596546173096, 2.2096827030181885, 2.212664842605591, 2.21038818359375, 2.208329916000366, 2.2099242210388184, 2.2072505950927734, 2.2073121070861816, 2.207967519760132, 2.2047789096832275, 2.20589542388916, 2.2046687602996826, 2.2038536071777344, 2.2040371894836426, 2.202902317047119, 2.2025651931762695, 2.2020668983459473, 2.201188087463379, 2.201261281967163, 2.199941396713257, 2.200051784515381, 2.1989798545837402, 2.199113607406616, 2.198185920715332, 2.1977908611297607, 2.197178363800049, 2.1970090866088867, 2.196171522140503, 2.195762872695923, 2.1951470375061035, 2.194765329360962, 2.1947755813598633, 2.1945981979370117, 2.195302724838257, 2.1960344314575195, 2.1999075412750244, 2.1993932723999023, 2.197763442993164, 2.192169666290283, 2.1915929317474365, 2.1934826374053955, 2.1944518089294434, 2.194420337677002, 2.1908934116363525, 2.189470052719116, 2.1905131340026855, 2.1928415298461914, 2.1942694187164307, 2.188389301300049, 2.1861581802368164, 2.1863648891448975, 2.187070369720459, 2.1897668838500977, 2.1911637783050537, 2.1963558197021484, 2.1979551315307617, 2.1876626014709473, 2.183931827545166, 2.1891322135925293, 2.1872365474700928, 2.1891894340515137, 2.1911418437957764, 2.1863694190979004, 2.18670916557312, 2.1884355545043945, 2.1933560371398926, 2.18381929397583, 2.1833717823028564, 2.183791399002075, 2.184979200363159, 2.1836163997650146, 2.1795358657836914, 2.1787281036376953, 2.1790430545806885, 2.1782724857330322, 2.183286190032959, 2.193866729736328, 2.2021687030792236, 2.1919939517974854, 2.185748815536499, 2.198596477508545, 2.189209461212158, 2.1829679012298584, 2.191635847091675, 2.1832311153411865, 2.177567481994629, 2.1849679946899414, 2.1764681339263916, 2.1783039569854736, 2.179903507232666, 2.1755592823028564, 2.1760497093200684, 2.1764512062072754, 2.1751651763916016, 2.1721956729888916, 2.1728310585021973, 2.1710562705993652, 2.1728062629699707, 2.1708903312683105, 2.1698062419891357, 2.171437978744507, 2.1687164306640625, 2.168283462524414, 2.1680004596710205, 2.1705470085144043, 2.184877634048462, 2.213331699371338, 2.19381046295166, 2.174678087234497, 2.1872639656066895, 2.1778948307037354, 2.1773953437805176, 2.178938388824463, 2.176454544067383, 2.17097806930542, 2.1760363578796387, 2.1729297637939453, 2.1721880435943604, 2.1741743087768555, 2.167182207107544, 2.1695871353149414, 2.164567708969116, 2.1701738834381104, 2.1636407375335693, 2.1674680709838867, 2.162656545639038, 2.1651315689086914, 2.161565065383911, 2.1616158485412598, 2.1603682041168213, 2.164405584335327, 2.178354024887085, 2.214104175567627, 2.198878049850464, 2.1797783374786377, 2.189596652984619, 2.1668219566345215, 2.180349349975586, 2.1671152114868164, 2.172537326812744, 2.1722640991210938, 2.165457010269165, 2.167869806289673, 2.1632227897644043, 2.166548013687134, 2.1627111434936523, 2.1625723838806152, 2.161372423171997, 2.160099983215332, 2.1590633392333984, 2.1563055515289307, 2.158090591430664, 2.1546576023101807, 2.153721809387207, 2.154416084289551, 2.1539783477783203, 2.157947063446045, 2.1702375411987305, 2.1856017112731934, 2.181173324584961, 2.15691876411438, 2.1813385486602783, 2.1647326946258545, 2.1601176261901855, 2.166351318359375, 2.1534388065338135, 2.1647465229034424, 2.1585237979888916, 2.156705141067505, 2.157369375228882, 2.1534037590026855, 2.153860569000244, 2.1537036895751953, 2.14994478225708, 2.152794599533081, 2.146907329559326, 2.14738392829895, 2.147470235824585, 2.1472768783569336, 2.1420836448669434, 2.1456403732299805, 2.1453142166137695, 2.144221305847168, 2.1429030895233154, 2.1443068981170654, 2.143415927886963, 2.150873899459839, 2.1786630153656006, 2.1831886768341064, 2.1649134159088135, 2.1459720134735107, 2.161992311477661, 2.1485068798065186, 2.144972801208496, 2.1515913009643555, 2.1442296504974365, 2.1446263790130615, 2.148179292678833, 2.139662265777588, 2.145341634750366, 2.1393513679504395, 2.1378064155578613, 2.1399619579315186, 2.138018846511841, 2.135887861251831, 2.131563663482666, 2.1360299587249756, 2.136530637741089, 2.1368601322174072, 2.1494204998016357, 2.167696952819824, 2.168705940246582, 2.156785011291504, 2.1351184844970703, 2.15720272064209, 2.1545767784118652, 2.144998073577881, 2.1364262104034424, 2.142059564590454, 2.1395986080169678, 2.1332309246063232, 2.133646011352539, 2.134502410888672, 2.137834310531616, 2.1326656341552734, 2.130025625228882, 2.126188278198242, 2.1270318031311035, 2.127129077911377, 2.1297669410705566, 2.1414756774902344, 2.1548380851745605, 2.157269239425659, 2.131901264190674, 2.1349024772644043, 2.13529896736145, 2.143192768096924, 2.1332476139068604, 2.1299219131469727, 2.1307902336120605, 2.132905960083008, 2.129791736602783, 2.123002767562866, 2.131756544113159, 2.1323204040527344, 2.1443839073181152, 2.1233603954315186, 2.1267635822296143, 2.135835886001587, 2.149479389190674, 2.1333980560302734, 2.132086753845215, 2.134124755859375, 2.135568380355835, 2.121403455734253, 2.1342129707336426, 2.1275992393493652, 2.126593828201294, 2.12227201461792, 2.1215457916259766, 2.122570276260376, 2.117948293685913, 2.1212289333343506, 2.1140270233154297, 2.1171300411224365, 2.113600254058838, 2.1160364151000977, 2.1241812705993652, 2.152449607849121, 2.2050254344940186, 2.1481175422668457, 2.157601833343506, 2.179713249206543, 2.128633737564087, 2.1537423133850098, 2.133202075958252, 2.139723062515259, 2.130186080932617, 2.133286476135254, 2.1302876472473145, 2.1261050701141357, 2.1270039081573486, 2.1208555698394775, 2.123706102371216, 2.121349573135376, 2.1143205165863037, 2.119502067565918, 2.115582227706909, 2.111546754837036, 2.1143176555633545, 2.113351583480835, 2.1101298332214355, 2.1075944900512695, 2.110435724258423, 2.1194019317626953, 2.1278700828552246, 2.12066912651062, 2.107605457305908, 2.102085828781128, 2.1097803115844727, 2.1156418323516846, 2.115705966949463, 2.111945390701294, 2.1038215160369873, 2.101853370666504, 2.110140562057495, 2.1213183403015137, 2.127279281616211, 2.109745740890503, 2.098485231399536, 2.1076953411102295, 2.1150248050689697, 2.1185929775238037, 2.114320755004883, 2.1018428802490234, 2.096930503845215, 2.102492332458496, 2.114607095718384, 2.1081905364990234, 2.093466281890869, 2.102752447128296, 2.115177631378174, 2.1356186866760254, 2.1326441764831543, 2.1036787033081055, 2.127619743347168, 2.147599697113037, 2.123325824737549, 2.127224922180176, 2.1186957359313965, 2.1131184101104736, 2.111211061477661, 2.1115312576293945, 2.1010324954986572, 2.108670711517334, 2.104952573776245, 2.103682518005371, 2.097161054611206, 2.1014087200164795, 2.0930728912353516, 2.102789878845215, 2.0996861457824707, 2.1135616302490234, 2.112847328186035, 2.0948469638824463, 2.0921831130981445, 2.091898202896118, 2.1083717346191406, 2.1125986576080322, 2.1073567867279053, 2.094599962234497, 2.0907623767852783, 2.098684787750244, 2.1037604808807373, 2.091801166534424, 2.086106300354004, 2.0839040279388428, 2.091001033782959, 2.094327926635742, 2.0894885063171387, 2.083256244659424, 2.0807971954345703, 2.081780433654785, 2.079643726348877, 2.079371690750122, 2.0837562084198, 2.096581220626831, 2.140653610229492, 2.1302309036254883, 2.0928120613098145, 2.1025373935699463, 2.1158554553985596, 2.102027177810669, 2.096066474914551, 2.0923056602478027, 2.0965256690979004, 2.0902516841888428, 2.0894899368286133, 2.099574089050293, 2.084092378616333, 2.085984468460083, 2.089916467666626, 2.080003499984741, 2.084320306777954, 2.0735204219818115, 2.0827808380126953, 2.079822301864624, 2.084975481033325, 2.0842790603637695, 2.0831847190856934, 2.0841822624206543, 2.0909788608551025, 2.1060409545898438, 2.0778260231018066, 2.083209276199341, 2.0830907821655273, 2.0802693367004395, 2.0984740257263184, 2.076921224594116, 2.0822641849517822, 2.090740203857422, 2.0940210819244385, 2.085394859313965, 2.066929340362549, 2.0766305923461914, 2.0922930240631104, 2.1053547859191895, 2.088106870651245, 2.0797476768493652, 2.103839159011841, 2.1057910919189453, 2.087745428085327, 2.086965799331665, 2.087528944015503, 2.0741357803344727, 2.07318377494812, 2.075418710708618, 2.0737111568450928, 2.066427230834961, 2.0750350952148438, 2.0907933712005615, 2.0890259742736816, 2.068603515625, 2.07572865486145, 2.0820236206054688, 2.0793099403381348, 2.0844578742980957, 2.062683343887329, 2.0768966674804688, 2.0887222290039062, 2.076605796813965, 2.0672695636749268, 2.06968355178833, 2.077810764312744, 2.0739378929138184, 2.055196523666382, 2.06766414642334, 2.0637929439544678, 2.0647506713867188, 2.0567779541015625, 2.052278518676758, 2.054816722869873, 2.0568225383758545, 2.0555272102355957, 2.062483549118042, 2.0668137073516846, 2.0578386783599854, 2.0536868572235107, 2.054626226425171, 2.0507805347442627, 2.0523123741149902, 2.0500545501708984, 2.0547449588775635, 2.062192440032959, 2.063570261001587, 2.054487705230713, 2.0563483238220215, 2.0489578247070312, 2.0473170280456543, 2.0425963401794434, 2.0463056564331055, 2.047823429107666, 2.0511460304260254, 2.05226469039917, 2.081200361251831, 2.107344388961792, 2.0853466987609863, 2.0490691661834717, 2.0904440879821777, 2.0897793769836426, 2.078575611114502, 2.081679582595825, 2.063951253890991, 2.0717904567718506, 2.0563628673553467, 2.069021463394165, 2.052197217941284, 2.05461049079895, 2.0555248260498047, 2.04233980178833, 2.048252820968628, 2.044348955154419, 2.040252685546875, 2.0478336811065674, 2.040163278579712, 2.043794631958008, 2.0440845489501953, 2.036210775375366, 2.0402626991271973, 2.0422306060791016, 2.0461666584014893, 2.0432639122009277, 2.046538829803467, 2.0462594032287598, 2.044124126434326, 2.030367851257324, 2.0269107818603516, 2.0310256481170654, 2.0304296016693115, 2.024731397628784, 2.031965970993042, 2.049686908721924, 2.0847718715667725, 2.0748467445373535]</t>
+  </si>
+  <si>
+    <t>[3.5095903873443604, 3.4489684104919434, 3.339707374572754, 3.162562608718872, 2.9825661182403564, 2.949648380279541, 2.8513505458831787, 2.786360263824463, 2.7651185989379883, 2.724621534347534, 2.6648411750793457, 2.605236291885376, 2.5667612552642822, 2.540367364883423, 2.4989113807678223, 2.4643256664276123, 2.4446396827697754, 2.4271960258483887, 2.408658266067505, 2.3920631408691406, 2.379755973815918, 2.36987042427063, 2.361659288406372, 2.3571841716766357, 2.3522145748138428, 2.3459131717681885, 2.342430353164673, 2.3393330574035645, 2.333306074142456, 2.328042984008789, 2.3236935138702393, 2.318352222442627, 2.3131792545318604, 2.3095407485961914, 2.305798053741455, 2.302851676940918, 2.3008761405944824, 2.297832489013672, 2.2941598892211914, 2.2913074493408203, 2.2881228923797607, 2.2848634719848633, 2.282146692276001, 2.279233932495117, 2.2768354415893555, 2.274467706680298, 2.2722373008728027, 2.2702736854553223, 2.268216133117676, 2.2661170959472656, 2.2639448642730713, 2.262059450149536, 2.2601139545440674, 2.258042097091675, 2.2562196254730225, 2.2544631958007812, 2.2526614665985107, 2.251073122024536, 2.2497000694274902, 2.2485225200653076, 2.249143362045288, 2.2541801929473877, 2.247641086578369, 2.245849847793579, 2.249382257461548, 2.2423505783081055, 2.2471234798431396, 2.243851661682129, 2.242658853530884, 2.243673086166382, 2.2394087314605713, 2.24165940284729, 2.2374486923217773, 2.2398855686187744, 2.2369229793548584, 2.2368404865264893, 2.236116647720337, 2.234091281890869, 2.235264778137207, 2.2325942516326904, 2.233319044113159, 2.2322986125946045, 2.2310378551483154, 2.2314419746398926, 2.231264591217041, 2.229811191558838, 2.229473829269409, 2.229574680328369, 2.227278232574463, 2.227938413619995, 2.227445363998413, 2.2258434295654297, 2.2254252433776855, 2.2259626388549805, 2.223963975906372, 2.223522901535034, 2.2639448642730713, 2.5532195568084717, 2.3088414669036865, 2.4003331661224365, 2.4282374382019043, 2.4083375930786133, 2.377146005630493, 2.348184108734131, 2.319197416305542, 2.2977774143218994, 2.2949070930480957, 2.3016788959503174, 2.301616907119751, 2.294124126434326, 2.2877039909362793, 2.285269021987915, 2.2848803997039795, 2.283351182937622, 2.279597043991089, 2.275336980819702, 2.273146152496338, 2.2731640338897705, 2.272822856903076, 2.269956588745117, 2.2657034397125244, 2.2625739574432373, 2.261650323867798, 2.2621212005615234, 2.262200355529785, 2.26108455657959, 2.259105920791626, 2.2570033073425293, 2.255444049835205, 2.2546331882476807, 2.254275321960449, 2.2538888454437256, 2.2531192302703857, 2.252072334289551, 2.2510251998901367, 2.2501089572906494, 2.249328374862671, 2.248750686645508, 2.248239517211914, 2.247509241104126, 2.2466037273406982, 2.245875120162964, 2.245373010635376, 2.244762897491455, 2.243967056274414, 2.2430503368377686, 2.2424652576446533, 2.2420248985290527, 2.24131178855896, 2.24052357673645, 2.2398643493652344, 2.2391984462738037, 2.2385313510894775, 2.2379000186920166, 2.2371649742126465, 2.2364919185638428, 2.2358486652374268, 2.2350645065307617, 2.2344415187835693, 2.23380970954895, 2.2330758571624756, 2.23242449760437, 2.231736421585083, 2.231100082397461, 2.230390787124634, 2.229759693145752, 2.22898268699646, 2.2282354831695557, 2.2274837493896484, 2.2266933917999268, 2.2259628772735596, 2.225234031677246, 2.224498987197876, 2.223719835281372, 2.2229340076446533, 2.2221293449401855, 2.221318483352661, 2.220510482788086, 2.2197446823120117, 2.219001054763794, 2.2183687686920166, 2.217881441116333, 2.2176690101623535, 2.2165563106536865, 2.215508460998535, 2.21453857421875, 2.213932991027832, 2.2135891914367676, 2.213380813598633, 2.21364688873291, 2.2121167182922363, 2.211120128631592, 2.209794759750366, 2.20898175239563, 2.2080955505371094, 2.2071990966796875, 2.2064712047576904, 2.2057173252105713, 2.204972505569458, 2.2041618824005127, 2.2036900520324707, 2.2069408893585205, 2.226145029067993, 2.20693302154541, 2.2162389755249023, 2.226309061050415, 2.2179360389709473, 2.2145745754241943, 2.216212034225464, 2.2061307430267334, 2.2166967391967773, 2.2061994075775146, 2.2059805393218994, 2.208207130432129, 2.203378915786743, 2.2047300338745117, 2.20182728767395, 2.2069408893585205, 2.5301125049591064, 2.365328311920166, 2.2727138996124268, 2.335324764251709, 2.283543348312378, 2.2571473121643066, 2.2637438774108887, 2.2667388916015625, 2.2564027309417725, 2.243823289871216, 2.2423155307769775, 2.2497494220733643, 2.2472996711730957, 2.2368838787078857, 2.233253002166748, 2.236078977584839, 2.2376656532287598, 2.2345004081726074, 2.2293701171875, 2.2278382778167725, 2.2298197746276855, 2.228259801864624, 2.223982572555542, 2.222849130630493, 2.2235324382781982, 2.2233059406280518, 2.221242666244507, 2.2193689346313477, 2.218719720840454, 2.2170069217681885, 2.2155826091766357, 2.2154839038848877, 2.21480131149292, 2.2136693000793457, 2.2136940956115723, 2.2128565311431885, 2.2110228538513184, 2.210294485092163, 2.209569215774536, 2.208954095840454, 2.208925247192383, 2.2077972888946533, 2.2072196006774902, 2.206376552581787, 2.2056751251220703, 2.2050247192382812, 2.2045750617980957, 2.2038538455963135, 2.203179121017456, 2.2023885250091553, 2.2020509243011475, 2.2012112140655518, 2.200793743133545, 2.1999363899230957, 2.199260950088501, 2.198871612548828, 2.1980154514312744, 2.1972925662994385, 2.197096586227417, 2.1966986656188965, 2.1954476833343506, 2.1950719356536865, 2.195186138153076, 2.194307327270508, 2.1935806274414062, 2.1924686431884766, 2.1919095516204834, 2.1920053958892822, 2.191754102706909, 2.191465377807617, 2.189765214920044, 2.188896417617798, 2.188774347305298, 2.1888654232025146, 2.1896369457244873, 2.1875686645507812, 2.1864469051361084, 2.185500383377075, 2.1854023933410645, 2.186663866043091, 2.187006711959839, 2.190098524093628, 2.183974266052246, 2.184262275695801, 2.1877553462982178, 2.1858065128326416, 2.1855006217956543, 2.1849489212036133, 2.1877546310424805, 2.180954694747925, 2.1830694675445557, 2.1812219619750977, 2.1803781986236572, 2.1801164150238037, 2.17913556098938, 2.1817002296447754, 2.178220510482788, 2.182683229446411, 2.1843113899230957, 2.187563896179199, 2.178250312805176, 2.182631492614746, 2.178056001663208, 2.178929090499878, 2.1771278381347656, 2.179028034210205, 2.1786985397338867, 2.177143096923828, 2.1758792400360107, 2.175520420074463, 2.1755850315093994, 2.1734485626220703, 2.173557996749878, 2.171347141265869, 2.1720879077911377, 2.1719205379486084, 2.173166275024414, 2.1751983165740967, 2.179082155227661, 2.1782078742980957, 2.1733295917510986, 2.169252872467041, 2.1719343662261963, 2.1807668209075928, 2.168674945831299, 2.1773667335510254, 2.1949663162231445, 2.172673463821411, 2.181381940841675, 2.18011212348938, 2.1733129024505615, 2.181309223175049, 2.173429012298584, 2.1758880615234375, 2.1695189476013184, 2.1720526218414307, 2.170776128768921, 2.1729869842529297, 2.1663074493408203, 2.1700398921966553, 2.1698131561279297, 2.165834903717041, 2.166447162628174, 2.165236473083496, 2.1642231941223145, 2.1637332439422607, 2.164686679840088, 2.160569190979004, 2.162958860397339, 2.168344497680664, 2.1665167808532715, 2.1611533164978027, 2.1579716205596924, 2.1657464504241943, 2.169355869293213, 2.1622138023376465, 2.157627820968628, 2.1734213829040527, 2.1664888858795166, 2.1600182056427, 2.1572070121765137, 2.16538405418396, 2.1624603271484375, 2.1544787883758545, 2.1572558879852295, 2.1636593341827393, 2.1551175117492676, 2.151677370071411, 2.154224157333374, 2.155978202819824, 2.1542723178863525, 2.1514506340026855, 2.148369312286377, 2.148293972015381, 2.149299144744873, 2.1543941497802734, 2.1696419715881348, 2.181535005569458, 2.1632027626037598, 2.152358293533325, 2.160721778869629, 2.1573779582977295, 2.148519992828369, 2.15364408493042, 2.152506113052368, 2.147461175918579, 2.148179769515991, 2.1481268405914307, 2.1496520042419434, 2.1461822986602783, 2.144287109375, 2.142348051071167, 2.141674041748047, 2.1440138816833496, 2.1502206325531006, 2.174715280532837, 2.195375442504883, 2.1631224155426025, 2.1646242141723633, 2.164527416229248, 2.151426076889038, 2.165300130844116, 2.149118423461914, 2.159247875213623, 2.148308515548706, 2.1530921459198, 2.150252103805542, 2.146155834197998, 2.1490235328674316, 2.1416585445404053, 2.1453938484191895, 2.140076160430908, 2.1407711505889893, 2.1415886878967285, 2.139336109161377, 2.13771653175354, 2.1358890533447266, 2.13689923286438, 2.1404144763946533, 2.142374038696289, 2.145580291748047, 2.147023916244507, 2.143685817718506, 2.133493661880493, 2.131273031234741, 2.1344218254089355, 2.138949394226074, 2.143622875213623, 2.1406445503234863, 2.1336779594421387, 2.127396583557129, 2.1293838024139404, 2.1370599269866943, 2.1433603763580322, 2.1405882835388184, 2.1305387020111084, 2.1241939067840576, 2.1297740936279297, 2.1386051177978516, 2.146782398223877, 2.1373941898345947, 2.1242384910583496, 2.1245436668395996, 2.132449150085449, 2.139458656311035, 2.134561061859131, 2.1237967014312744, 2.1260123252868652, 2.134965419769287, 2.1410138607025146, 2.1320641040802, 2.1240758895874023, 2.1225883960723877, 2.1281068325042725, 2.1348214149475098, 2.126014471054077, 2.125047206878662, 2.118008613586426, 2.121150016784668, 2.126157760620117, 2.1245737075805664, 2.131290912628174, 2.122441053390503, 2.1217498779296875, 2.1157443523406982, 2.1128101348876953, 2.1144843101501465, 2.111067533493042, 2.1108505725860596, 2.115529775619507, 2.129072904586792, 2.1791601181030273, 2.195969820022583, 2.13006329536438, 2.169529914855957, 2.143906593322754, 2.15266752243042, 2.132450580596924, 2.1495559215545654, 2.1238276958465576, 2.1455509662628174, 2.1242618560791016, 2.1367523670196533, 2.1229214668273926, 2.127098321914673, 2.1244394779205322, 2.1212332248687744, 2.121490716934204, 2.1161465644836426, 2.1192851066589355, 2.1127536296844482, 2.117295742034912, 2.1086790561676025, 2.114868640899658, 2.109323263168335, 2.111295700073242, 2.109764575958252, 2.1117732524871826, 2.1186890602111816, 2.136911630630493, 2.152604341506958, 2.114191770553589, 2.1209018230438232, 2.1383681297302246, 2.1252167224884033, 2.1117396354675293, 2.1318981647491455, 2.1118836402893066, 2.112567901611328, 2.116302251815796, 2.110776662826538, 2.103874921798706, 2.109625816345215, 2.10699725151062, 2.1021931171417236, 2.1005160808563232, 2.104747772216797, 2.10615611076355, 2.106663465499878, 2.107311248779297, 2.1058168411254883, 2.1062350273132324, 2.0992250442504883, 2.0976169109344482, 2.0941591262817383, 2.092508554458618, 2.0939393043518066, 2.0958847999572754, 2.1124963760375977, 2.1562256813049316, 2.1472814083099365, 2.102743625640869, 2.123750925064087, 2.1258544921875, 2.0985066890716553, 2.120676040649414, 2.107445240020752, 2.1010212898254395, 2.1136488914489746, 2.0974695682525635, 2.1004836559295654, 2.1003470420837402, 2.095675468444824, 2.0985000133514404, 2.09077787399292, 2.10060453414917, 2.089771032333374, 2.0914998054504395, 2.089956760406494, 2.087023973464966, 2.090195655822754, 2.08686900138855, 2.0958809852600098, 2.1149396896362305, 2.15238094329834, 2.1408302783966064, 2.095428943634033, 2.1263389587402344, 2.111542224884033, 2.098390579223633, 2.1047732830047607, 2.101625442504883, 2.0917701721191406, 2.103689193725586, 2.0892832279205322, 2.091545820236206, 2.0930697917938232, 2.0884528160095215, 2.0843889713287354, 2.091031551361084, 2.083465099334717, 2.083726644515991, 2.080430507659912, 2.0802955627441406, 2.083679676055908, 2.0815269947052, 2.0850119590759277, 2.0789785385131836, 2.0826714038848877, 2.0841522216796875]</t>
+  </si>
+  <si>
+    <t>[3.5142710208892822, 3.462247371673584, 3.3682453632354736, 3.2091825008392334, 3.013458251953125, 2.952646255493164, 2.887021780014038, 2.799901247024536, 2.772658586502075, 2.745555877685547, 2.696441888809204, 2.639683246612549, 2.5905022621154785, 2.5604937076568604, 2.532090663909912, 2.4916417598724365, 2.463038444519043, 2.4496536254882812, 2.4379048347473145, 2.4246325492858887, 2.411003351211548, 2.3974556922912598, 2.3871896266937256, 2.3771605491638184, 2.3682894706726074, 2.3622772693634033, 2.3571290969848633, 2.3524911403656006, 2.3489859104156494, 2.345475673675537, 2.3399033546447754, 2.3334763050079346, 2.3288135528564453, 2.325159788131714, 2.3212950229644775, 2.3173725605010986, 2.3139569759368896, 2.310805082321167, 2.307936906814575, 2.305229425430298, 2.302067279815674, 2.2987992763519287, 2.2960987091064453, 2.2934505939483643, 2.29042911529541, 2.287623882293701, 2.2847306728363037, 2.2820639610290527, 2.279397964477539, 2.2769737243652344, 2.274641513824463, 2.2723915576934814, 2.2699038982391357, 2.267568588256836, 2.265125274658203, 2.2627835273742676, 2.2607421875, 2.2590863704681396, 2.257643938064575, 2.2567265033721924, 2.2565293312072754, 2.256089210510254, 2.2555434703826904, 2.2529690265655518, 2.252586841583252, 2.2533960342407227, 2.2517967224121094, 2.250243902206421, 2.250420331954956, 2.2499747276306152, 2.2490336894989014, 2.2483036518096924, 2.248443841934204, 2.248094081878662, 2.247134208679199, 2.2465038299560547, 2.2466745376586914, 2.2464218139648438, 2.245914936065674, 2.245065689086914, 2.2445833683013916, 2.2445271015167236, 2.2444515228271484, 2.244495153427124, 2.243988037109375, 2.2434067726135254, 2.2424330711364746, 2.241922378540039, 2.2417550086975098, 2.2416493892669678, 2.241488456726074, 2.2409558296203613, 2.240497350692749, 2.239654302597046, 2.2390878200531006, 2.2386314868927, 2.238239288330078, 2.2380943298339844, 2.2381668090820312, 2.2393453121185303, 2.2397868633270264, 2.2407073974609375, 2.2365925312042236, 2.235227346420288, 2.2369983196258545, 2.2355098724365234, 2.2335927486419678, 2.2335610389709473, 2.2340281009674072, 2.234036922454834, 2.2315192222595215, 2.232530117034912, 2.2335221767425537, 2.2317185401916504, 2.2294249534606934, 2.2310497760772705, 2.229830503463745, 2.228471279144287, 2.2269866466522217, 2.227630138397217, 2.2295103073120117, 2.226801633834839, 2.2259867191314697, 2.2254443168640137, 2.2268447875976562, 2.2252144813537598, 2.2246081829071045, 2.2226932048797607, 2.222446918487549, 2.221500873565674, 2.2213354110717773, 2.2210071086883545, 2.2207515239715576, 2.2221713066101074, 2.226689577102661, 2.2289021015167236, 2.2277164459228516, 2.21950101852417, 2.223503351211548, 2.226900815963745, 2.2177886962890625, 2.2272732257843018, 2.228531837463379, 2.2207093238830566, 2.229889154434204, 2.2199363708496094, 2.223766565322876, 2.218210220336914, 2.2205822467803955, 2.219015121459961, 2.218003749847412, 2.2198843955993652, 2.2172272205352783, 2.2172305583953857, 2.215348482131958, 2.2162184715270996, 2.2149460315704346, 2.214277505874634, 2.214118242263794, 2.213557004928589, 2.212735891342163, 2.2131338119506836, 2.212327003479004, 2.210659980773926, 2.212402820587158, 2.2111029624938965, 2.210951566696167, 2.20963454246521, 2.2108559608459473, 2.208648920059204, 2.2091116905212402, 2.208268165588379, 2.2096872329711914, 2.211108684539795, 2.212703227996826, 2.2123706340789795, 2.208944797515869, 2.207298755645752, 2.2080235481262207, 2.2089314460754395, 2.208970069885254, 2.2070984840393066, 2.205374240875244, 2.205094337463379, 2.2048232555389404, 2.2051968574523926, 2.20710825920105, 2.2129504680633545, 2.219930410385132, 2.2171030044555664, 2.204913377761841, 2.2098746299743652, 2.2141366004943848, 2.2045302391052246, 2.2114946842193604, 2.211970329284668, 2.203594446182251, 2.2127997875213623, 2.2045302391052246, 2.788602113723755, 2.3477210998535156, 2.3271398544311523, 2.324373483657837, 2.3579869270324707, 2.368914842605591, 2.3454782962799072, 2.3141379356384277, 2.295079469680786, 2.285740375518799, 2.2797865867614746, 2.2746691703796387, 2.269890546798706, 2.265798568725586, 2.2634217739105225, 2.2623543739318848, 2.26104474067688, 2.2585041522979736, 2.2552621364593506, 2.2525763511657715, 2.2511284351348877, 2.25024151802063, 2.248431444168091, 2.2455673217773438, 2.24281907081604, 2.241124153137207, 2.240514039993286, 2.2402966022491455, 2.239835262298584, 2.2387402057647705, 2.236954689025879, 2.2347474098205566, 2.2326221466064453, 2.2309327125549316, 2.2296574115753174, 2.228572130203247, 2.227620840072632, 2.2267823219299316, 2.226057291030884, 2.2253975868225098, 2.224543809890747, 2.223489761352539, 2.222433567047119, 2.221438407897949, 2.2206778526306152, 2.2199578285217285, 2.218965530395508, 2.2179689407348633, 2.217156410217285, 2.2164723873138428, 2.2157227993011475, 2.214909315109253, 2.214223623275757, 2.213550329208374, 2.2129242420196533, 2.212225914001465, 2.211503505706787, 2.210832357406616, 2.2102560997009277, 2.209644079208374, 2.2090461254119873, 2.208488702774048, 2.2079241275787354, 2.207402467727661, 2.2068827152252197, 2.2063686847686768, 2.205878734588623, 2.2053394317626953, 2.2048895359039307, 2.2043657302856445, 2.203880548477173, 2.2034249305725098, 2.20293927192688, 2.2025647163391113, 2.202291488647461, 2.2023472785949707, 2.202777862548828, 2.2032036781311035, 2.2026796340942383, 2.200878143310547, 2.1995389461517334, 2.1995532512664795, 2.200333595275879, 2.200955867767334, 2.2003285884857178, 2.1987855434417725, 2.1972856521606445, 2.1969029903411865, 2.1974246501922607, 2.1984541416168213, 2.1997931003570557, 2.1996355056762695, 2.198310613632202, 2.195565938949585, 2.1940720081329346, 2.1944241523742676, 2.1958096027374268, 2.197831869125366, 2.1975667476654053, 2.196096181869507, 2.1931066513061523, 2.1914584636688232, 2.191547393798828, 2.1928951740264893, 2.19599986076355, 2.1989552974700928, 2.2007477283477783, 2.193652391433716, 2.1893720626831055, 2.1922497749328613, 2.1951491832733154, 2.192788600921631, 2.188183307647705, 2.1893696784973145, 2.193134307861328, 2.193939447402954, 2.1913087368011475, 2.1867659091949463, 2.186404228210449, 2.1888983249664307, 2.1916797161102295, 2.1942713260650635, 2.191974401473999, 2.1873056888580322, 2.185675621032715, 2.185351610183716, 2.1898725032806396, 2.192800521850586, 2.1972124576568604, 2.1916863918304443, 2.185241460800171, 2.18399715423584, 2.190279960632324, 2.1890320777893066, 2.1836819648742676, 2.1843132972717285, 2.184985876083374, 2.187668800354004, 2.1897401809692383, 2.181896448135376, 2.1879308223724365, 2.182286500930786, 2.1855313777923584, 2.1895763874053955, 2.181922674179077, 2.1847970485687256, 2.181091070175171, 2.180427312850952, 2.1820461750030518, 2.1793341636657715, 2.179466485977173, 2.18255615234375, 2.1838583946228027, 2.2001900672912598, 2.2318732738494873, 2.198648691177368, 2.195673704147339, 2.2034900188446045, 2.183187484741211, 2.207188606262207, 2.1843035221099854, 2.194876194000244, 2.188352108001709, 2.192298412322998, 2.1839680671691895, 2.1910085678100586, 2.1826164722442627, 2.1868128776550293, 2.1828773021698, 2.1853601932525635, 2.180575370788574, 2.181453227996826, 2.1824257373809814, 2.1786105632781982, 2.1792306900024414, 2.180091619491577, 2.1766746044158936, 2.178205728530884, 2.177161455154419, 2.1752514839172363, 2.1766064167022705, 2.175265312194824, 2.1740825176239014, 2.173929452896118, 2.1736245155334473, 2.1743643283843994, 2.1741931438446045, 2.1737451553344727, 2.177152633666992, 2.179703950881958, 2.1875522136688232, 2.18737530708313, 2.189767837524414, 2.1723246574401855, 2.1892971992492676, 2.191304922103882, 2.190080404281616, 2.175840377807617, 2.1846272945404053, 2.17578387260437, 2.179471731185913, 2.17575740814209, 2.179626703262329, 2.172529935836792, 2.177950859069824, 2.1718802452087402, 2.1767523288726807, 2.171139717102051, 2.175633668899536, 2.170433521270752, 2.173234224319458, 2.170179605484009, 2.171964406967163, 2.169541597366333, 2.1707608699798584, 2.1686782836914062, 2.169631242752075, 2.169246196746826, 2.1702311038970947, 2.1757073402404785, 2.1868906021118164, 2.1970486640930176, 2.174471616744995, 2.1754305362701416, 2.178901195526123, 2.17878794670105, 2.171671152114868, 2.1742355823516846, 2.1740288734436035, 2.1684608459472656, 2.17217755317688, 2.1696813106536865, 2.1709771156311035, 2.1681461334228516, 2.1695313453674316, 2.1699435710906982, 2.1673011779785156, 2.1684181690216064, 2.1662819385528564, 2.1679816246032715, 2.1678953170776367, 2.1662564277648926, 2.167901039123535, 2.1649794578552246, 2.1657090187072754, 2.1655263900756836, 2.164707899093628, 2.1641182899475098, 2.165090560913086, 2.1644654273986816, 2.1648221015930176, 2.1697306632995605, 2.1926167011260986, 2.217104911804199, 2.200057029724121, 2.167990207672119, 2.1958868503570557, 2.176754951477051, 2.1831233501434326, 2.1776692867279053, 2.17623233795166, 2.1772358417510986, 2.1732585430145264, 2.176011085510254, 2.1717476844787598, 2.1758148670196533, 2.170140266418457, 2.173853874206543, 2.168609857559204, 2.172539710998535, 2.1680285930633545, 2.170518159866333, 2.167830467224121, 2.1671879291534424, 2.1689209938049316, 2.1652333736419678, 2.166961193084717, 2.166081666946411, 2.1640238761901855, 2.166029453277588, 2.164882183074951, 2.16294527053833, 2.164515733718872, 2.164738655090332, 2.1633360385894775, 2.1618590354919434, 2.1632587909698486, 2.1640207767486572, 2.1633293628692627, 2.161958694458008, 2.161468982696533, 2.1614274978637695, 2.1622540950775146, 2.163241386413574, 2.1639926433563232, 2.1645874977111816, 2.16483998298645, 2.1646387577056885, 2.1642322540283203, 2.1625185012817383, 2.160937786102295, 2.1601927280426025, 2.1599862575531006, 2.1602115631103516, 2.160393714904785, 2.1613075733184814, 2.1633551120758057, 2.1658923625946045, 2.168184757232666, 2.168102264404297, 2.1655545234680176, 2.163276433944702, 2.159881114959717, 2.160186290740967, 2.1630983352661133, 2.1633994579315186, 2.161951780319214, 2.1598148345947266, 2.159273862838745, 2.1597437858581543, 2.1596930027008057, 2.160313844680786, 2.1617395877838135, 2.1628928184509277, 2.1634459495544434, 2.161757469177246, 2.1602909564971924, 2.160050868988037, 2.1599929332733154, 2.1603660583496094, 2.1586482524871826, 2.1575725078582764, 2.157435655593872, 2.158290147781372, 2.16031813621521, 2.1615283489227295, 2.166330099105835, 2.1737546920776367, 2.1779885292053223, 2.1701385974884033, 2.1584229469299316, 2.1630682945251465, 2.1690778732299805, 2.1595611572265625, 2.1614954471588135, 2.166288375854492, 2.158646583557129, 2.1607449054718018, 2.164595365524292, 2.158020496368408, 2.1591238975524902, 2.163356304168701, 2.1578938961029053, 2.1578545570373535, 2.16098690032959, 2.1581709384918213, 2.156186580657959, 2.158202886581421, 2.1586952209472656, 2.1567542552948, 2.1560821533203125, 2.157740354537964, 2.162027359008789, 2.162794589996338, 2.1669180393218994, 2.161733627319336, 2.1651434898376465, 2.1643621921539307, 2.1562652587890625, 2.1576616764068604, 2.1633927822113037, 2.1589276790618896, 2.1557271480560303, 2.1586339473724365, 2.1582837104797363, 2.155590772628784, 2.1559882164001465, 2.15681791305542, 2.1559929847717285, 2.1544182300567627, 2.1547160148620605, 2.1566648483276367, 2.1570611000061035, 2.157900333404541, 2.1577510833740234, 2.161837339401245, 2.168797016143799, 2.167576313018799, 2.1625449657440186, 2.158179759979248, 2.1566901206970215, 2.1592938899993896, 2.1598153114318848, 2.1570303440093994, 2.1550819873809814, 2.155238151550293, 2.157989025115967, 2.1600863933563232, 2.1552581787109375, 2.1538188457489014, 2.1554527282714844, 2.154679775238037, 2.154407501220703, 2.1558194160461426, 2.1569771766662598, 2.1569466590881348, 2.1550891399383545, 2.1546459197998047, 2.155930757522583, 2.1549935340881348, 2.15419602394104, 2.153061866760254, 2.153998374938965, 2.1564486026763916, 2.157808542251587, 2.159029722213745, 2.158005475997925, 2.1592273712158203, 2.1630561351776123, 2.156442880630493, 2.1523125171661377, 2.15261173248291, 2.1550867557525635, 2.1570446491241455, 2.1570425033569336, 2.15909743309021, 2.161403179168701, 2.1556930541992188, 2.151369333267212, 2.152993679046631, 2.154999017715454, 2.154916286468506, 2.1546990871429443, 2.155672788619995, 2.157057285308838, 2.1523489952087402, 2.151947021484375, 2.1553306579589844, 2.1526312828063965, 2.1501190662384033, 2.1507623195648193, 2.1517527103424072, 2.1520626544952393, 2.1514546871185303, 2.1530964374542236, 2.1594784259796143, 2.170541524887085, 2.168309211730957, 2.158322811126709, 2.1521499156951904, 2.1599698066711426, 2.1617987155914307, 2.151785373687744, 2.1581945419311523, 2.163090705871582, 2.152034044265747, 2.154984951019287, 2.1609952449798584, 2.1520681381225586, 2.1544089317321777, 2.162468194961548, 2.1527767181396484, 2.1523337364196777, 2.1569876670837402, 2.1527817249298096, 2.14967679977417, 2.1523706912994385, 2.1521494388580322, 2.1487410068511963, 2.1496493816375732, 2.150531768798828, 2.1512575149536133, 2.1494929790496826, 2.1477348804473877, 2.1486623287200928, 2.1501851081848145, 2.1512887477874756, 2.1523373126983643, 2.1531777381896973, 2.15215802192688, 2.1494410037994385, 2.149369716644287, 2.1529507637023926, 2.1590864658355713, 2.1561343669891357, 2.1502773761749268, 2.149897575378418, 2.1527280807495117, 2.1544015407562256, 2.1490964889526367, 2.1476759910583496, 2.1512246131896973, 2.1502363681793213, 2.147770881652832, 2.1472833156585693, 2.1487488746643066, 2.1518561840057373, 2.151179075241089, 2.1509406566619873, 2.1547553539276123, 2.1532907485961914, 2.1515767574310303, 2.148542881011963, 2.1458401679992676, 2.1493613719940186, 2.15179705619812, 2.1539478302001953, 2.150425910949707, 2.1477017402648926, 2.1489298343658447, 2.146113157272339, 2.1454784870147705, 2.1477270126342773, 2.1476070880889893, 2.1513049602508545, 2.1524927616119385, 2.1508190631866455, 2.154294729232788, 2.153008460998535, 2.147155284881592, 2.1478376388549805, 2.1468820571899414, 2.1530606746673584, 2.149695873260498, 2.149848222732544, 2.150092601776123, 2.1470649242401123, 2.1465837955474854, 2.1438510417938232, 2.1454334259033203, 2.145840883255005, 2.145282506942749, 2.1478991508483887, 2.150635242462158, 2.1538307666778564, 2.152456521987915, 2.145704984664917, 2.14451265335083, 2.1472201347351074, 2.1480984687805176, 2.1483347415924072, 2.145259141921997, 2.1436877250671387, 2.143989324569702, 2.144129991531372, 2.1454553604125977, 2.1459109783172607, 2.1477770805358887, 2.150927782058716, 2.151848793029785, 2.147061347961426, 2.1419286727905273, 2.142025947570801, 2.145791530609131, 2.1489264965057373, 2.1446094512939453, 2.1438355445861816, 2.1461801528930664, 2.145636558532715, 2.1428275108337402, 2.141479015350342, 2.1434688568115234, 2.144998788833618, 2.143507957458496, 2.143490791320801, 2.151383399963379, 2.158637046813965, 2.1516408920288086, 2.146462917327881, 2.148613214492798, 2.1509933471679688, 2.143080472946167, 2.1482901573181152, 2.143754005432129, 2.1458165645599365, 2.1452531814575195, 2.144468069076538, 2.1434175968170166, 2.1405560970306396, 2.144449234008789, 2.1442205905914307, 2.1430680751800537, 2.144437789916992, 2.141629457473755, 2.141496419906616, 2.1417977809906006, 2.138396739959717, 2.1419169902801514, 2.140073537826538, 2.140363931655884, 2.1433584690093994, 2.147212028503418, 2.158531665802002, 2.1565637588500977, 2.1489949226379395, 2.151684522628784, 2.1541800498962402, 2.151813507080078, 2.1514484882354736, 2.1488277912139893, 2.147190809249878, 2.14793062210083, 2.1508967876434326, 2.144709348678589, 2.145426034927368, 2.144166946411133, 2.14223575592041, 2.1431751251220703, 2.1431350708007812, 2.1404173374176025, 2.1419975757598877, 2.1475627422332764, 2.1413681507110596, 2.140491008758545, 2.1412153244018555, 2.140587091445923, 2.1376566886901855, 2.1384117603302, 2.1383426189422607, 2.136791467666626, 2.1359643936157227, 2.137751340866089, 2.1358561515808105, 2.135683298110962, 2.1348302364349365, 2.135446548461914, 2.1387228965759277, 2.1481881141662598, 2.1586995124816895, 2.168450117111206, 2.150935649871826, 2.1623241901397705, 2.1516504287719727, 2.149482488632202, 2.1502389907836914, 2.1421072483062744, 2.150670289993286, 2.138287305831909, 2.145578145980835, 2.141805410385132, 2.140841484069824, 2.1402313709259033, 2.1417055130004883, 2.139375925064087, 2.1383731365203857, 2.138763427734375, 2.1359593868255615, 2.1373813152313232, 2.1365301609039307, 2.135770320892334, 2.1337451934814453, 2.1347742080688477, 2.1353445053100586, 2.1334049701690674, 2.1342296600341797, 2.132584810256958, 2.1347830295562744, 2.1353485584259033, 2.1381587982177734, 2.1412041187286377, 2.146559000015259, 2.144193649291992, 2.13454008102417, 2.135145902633667, 2.1391496658325195, 2.1414878368377686, 2.1406373977661133, 2.139601945877075, 2.132629156112671, 2.132205009460449, 2.1350295543670654, 2.136950969696045, 2.1337761878967285, 2.134139060974121, 2.134890079498291, 2.1332807540893555, 2.1303954124450684, 2.1311542987823486, 2.132871627807617, 2.1290345191955566, 2.130225658416748, 2.130040168762207, 2.1305148601531982, 2.1310582160949707, 2.1300132274627686, 2.1320955753326416, 2.1434409618377686, 2.1688241958618164, 2.148160457611084, 2.145925760269165, 2.1540908813476562, 2.1443891525268555, 2.1457035541534424, 2.141282558441162, 2.144106149673462, 2.140254020690918, 2.1346919536590576, 2.141840934753418, 2.1338868141174316, 2.136723279953003, 2.134984016418457, 2.1359925270080566, 2.133896589279175, 2.132687568664551, 2.132045030593872, 2.1320321559906006, 2.1317169666290283, 2.1299753189086914, 2.1317501068115234, 2.128891944885254, 2.1312873363494873, 2.130289316177368, 2.1316657066345215, 2.1324846744537354, 2.1329944133758545, 2.136000156402588, 2.1325442790985107, 2.1298487186431885, 2.126981019973755, 2.127681255340576, 2.131007194519043, 2.132336378097534, 2.1381494998931885, 2.136042356491089, 2.135310649871826, 2.130110025405884, 2.1256966590881348, 2.127392292022705, 2.1299688816070557, 2.133120536804199, 2.130366086959839, 2.1272966861724854, 2.125898599624634, 2.1246566772460938, 2.1244921684265137, 2.12399959564209, 2.1243228912353516, 2.1277592182159424, 2.136857748031616, 2.138873815536499, 2.13435959815979, 2.1263840198516846, 2.125514507293701, 2.1302695274353027, 2.1326067447662354, 2.1304681301116943, 2.1279537677764893, 2.1271262168884277, 2.12876558303833, 2.1297385692596436, 2.130929946899414, 2.132619857788086, 2.1258809566497803, 2.1226613521575928, 2.1267669200897217, 2.128537654876709, 2.1282453536987305, 2.12930965423584, 2.130842685699463, 2.1269993782043457, 2.1213552951812744, 2.1225738525390625, 2.125964403152466, 2.1270205974578857, 2.1287038326263428, 2.1295578479766846, 2.1276609897613525, 2.123957633972168, 2.121295928955078, 2.121755838394165, 2.1212246417999268, 2.1203978061676025, 2.1212661266326904, 2.1242899894714355, 2.13187837600708, 2.1388981342315674, 2.133885622024536, 2.1264336109161377, 2.12630295753479, 2.126617431640625, 2.130591869354248, 2.1358802318573, 2.1198770999908447, 2.1278815269470215, 2.1374664306640625, 2.1273648738861084, 2.1331188678741455, 2.130368947982788, 2.137425661087036, 2.145204782485962, 2.1257472038269043, 2.1380064487457275, 2.135897397994995, 2.1356048583984375, 2.1254734992980957, 2.1317505836486816, 2.123392343521118, 2.126337766647339, 2.1256070137023926, 2.127910614013672, 2.123826026916504, 2.121910572052002, 2.1253421306610107, 2.1244094371795654, 2.12308931350708, 2.119616985321045, 2.121736764907837, 2.1216845512390137, 2.11972975730896, 2.1184327602386475, 2.11592173576355, 2.1178886890411377, 2.1172313690185547, 2.123016357421875, 2.119309663772583, 2.1216628551483154, 2.119640827178955, 2.11879825592041, 2.1181085109710693, 2.1153910160064697, 2.1137936115264893, 2.1133763790130615, 2.115325927734375, 2.115877389907837, 2.1187801361083984, 2.1281943321228027, 2.145580530166626, 2.128021478652954, 2.116427183151245, 2.1326751708984375, 2.1266729831695557, 2.1177866458892822, 2.122302532196045, 2.1248221397399902, 2.1207234859466553, 2.1175220012664795, 2.124000072479248, 2.1160006523132324, 2.1166763305664062, 2.120603561401367, 2.117957592010498, 2.1141767501831055, 2.113664150238037, 2.1199405193328857, 2.113872766494751, 2.112534999847412, 2.111337661743164, 2.113013744354248, 2.1161231994628906, 2.112034797668457, 2.1112139225006104, 2.109017848968506, 2.10969614982605, 2.1104021072387695, 2.115420341491699, 2.1205191612243652, 2.1242692470550537, 2.133662700653076, 2.122365951538086, 2.1209537982940674, 2.1302387714385986, 2.124241590499878, 2.1198740005493164, 2.122342348098755, 2.120387315750122, 2.1274254322052, 2.120870351791382, 2.1205246448516846, 2.1160318851470947, 2.115838050842285, 2.114433526992798, 2.113957405090332, 2.1116819381713867, 2.1126034259796143, 2.1108341217041016, 2.1092891693115234, 2.109264850616455, 2.1082890033721924, 2.1081795692443848, 2.1076431274414062, 2.106773614883423, 2.1081717014312744, 2.1049389839172363, 2.106128692626953, 2.105882406234741, 2.110717296600342, 2.129084825515747, 2.1488938331604004, 2.131256580352783, 2.114152193069458, 2.1285440921783447, 2.1205618381500244, 2.108780860900879, 2.1214940547943115, 2.11120343208313, 2.1141538619995117, 2.111828565597534, 2.110872268676758, 2.1081724166870117, 2.108935832977295, 2.109304904937744, 2.104613780975342, 2.10782527923584, 2.1057300567626953, 2.1069042682647705, 2.1051063537597656, 2.1041951179504395, 2.105881929397583, 2.103653907775879, 2.1034512519836426, 2.104583263397217, 2.1053271293640137, 2.111539602279663, 2.1176693439483643, 2.1322169303894043, 2.1192739009857178, 2.106400728225708, 2.1308469772338867, 2.1172103881835938, 2.108515977859497, 2.1129586696624756, 2.1096279621124268, 2.104146718978882, 2.106982469558716, 2.1053836345672607, 2.106405735015869, 2.103912353515625, 2.1063296794891357, 2.1086206436157227, 2.1022775173187256, 2.1058218479156494, 2.1075599193573, 2.1048436164855957, 2.108523368835449, 2.1040279865264893, 2.103783130645752, 2.109299659729004, 2.0988199710845947, 2.1076948642730713, 2.1033763885498047, 2.1055843830108643, 2.113189935684204, 2.1223809719085693, 2.115316152572632, 2.114262819290161, 2.103241443634033, 2.1146774291992188, 2.112248420715332, 2.1218221187591553, 2.10665225982666, 2.1107192039489746, 2.1039462089538574, 2.1132311820983887, 2.1055285930633545, 2.1118266582489014, 2.107539653778076, 2.104445695877075, 2.10261869430542, 2.1016011238098145, 2.1003506183624268, 2.102532386779785, 2.1029305458068848, 2.102614402770996, 2.1029789447784424, 2.1044769287109375, 2.104245901107788, 2.1011157035827637, 2.097151756286621, 2.0980777740478516, 2.1092324256896973, 2.108884811401367, 2.100677967071533, 2.099557399749756, 2.1044223308563232, 2.1054584980010986, 2.105644941329956, 2.101417303085327, 2.098374128341675, 2.102200746536255, 2.1087944507598877, 2.109269142150879, 2.102098226547241, 2.1002793312072754, 2.104990243911743, 2.1101362705230713, 2.0984346866607666, 2.1050336360931396, 2.1118359565734863, 2.1068427562713623, 2.1021475791931152, 2.1202468872070312, 2.0977659225463867, 2.109571933746338, 2.111515522003174, 2.100771427154541, 2.119982957839966, 2.1019394397735596, 2.108963966369629, 2.1041131019592285, 2.0991370677948, 2.10609769821167, 2.0951616764068604, 2.1089186668395996, 2.096102476119995, 2.1022045612335205, 2.0957953929901123, 2.0968496799468994, 2.0990757942199707, 2.0943055152893066, 2.098961353302002, 2.100309371948242, 2.092592716217041, 2.1017141342163086, 2.0975735187530518, 2.096621513366699, 2.1021430492401123, 2.098893880844116, 2.100970506668091, 2.10526704788208, 2.1069788932800293, 2.1101372241973877, 2.1023411750793457, 2.113581657409668]</t>
   </si>
 </sst>
 </file>
@@ -470,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1829,10 +1856,169 @@
         <v>30</v>
       </c>
       <c r="Q30" t="s">
+        <v>34</v>
+      </c>
+      <c r="R30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>14</v>
+      </c>
+      <c r="E31">
+        <v>100</v>
+      </c>
+      <c r="F31">
+        <v>0.01</v>
+      </c>
+      <c r="G31">
+        <v>0.01</v>
+      </c>
+      <c r="H31">
+        <v>0.01</v>
+      </c>
+      <c r="I31">
+        <v>0.001</v>
+      </c>
+      <c r="J31">
+        <v>10000</v>
+      </c>
+      <c r="K31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" t="s">
+        <v>22</v>
+      </c>
+      <c r="M31">
+        <v>0.3224606513977051</v>
+      </c>
+      <c r="N31">
+        <v>0.3340963423252106</v>
+      </c>
+      <c r="P31" t="s">
         <v>31</v>
       </c>
-      <c r="R30" t="s">
+      <c r="Q31" t="s">
+        <v>35</v>
+      </c>
+      <c r="R31" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32">
+        <v>14</v>
+      </c>
+      <c r="E32">
+        <v>100</v>
+      </c>
+      <c r="F32">
+        <v>0.01</v>
+      </c>
+      <c r="G32">
+        <v>0.01</v>
+      </c>
+      <c r="H32">
+        <v>0.01</v>
+      </c>
+      <c r="I32">
+        <v>0.001</v>
+      </c>
+      <c r="J32">
+        <v>10000</v>
+      </c>
+      <c r="K32" t="s">
+        <v>20</v>
+      </c>
+      <c r="L32" t="s">
+        <v>22</v>
+      </c>
+      <c r="M32">
+        <v>0.3210300505161285</v>
+      </c>
+      <c r="N32">
+        <v>0.3282784819602966</v>
+      </c>
+      <c r="P32" t="s">
         <v>32</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>36</v>
+      </c>
+      <c r="R32" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33">
+        <v>14</v>
+      </c>
+      <c r="E33">
+        <v>100</v>
+      </c>
+      <c r="F33">
+        <v>0.98</v>
+      </c>
+      <c r="G33">
+        <v>0.01</v>
+      </c>
+      <c r="H33">
+        <v>0.01</v>
+      </c>
+      <c r="I33">
+        <v>0.001</v>
+      </c>
+      <c r="J33">
+        <v>10000</v>
+      </c>
+      <c r="K33" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" t="s">
+        <v>22</v>
+      </c>
+      <c r="M33">
+        <v>0.343633770942688</v>
+      </c>
+      <c r="N33">
+        <v>0.3377004563808441</v>
+      </c>
+      <c r="P33" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>37</v>
+      </c>
+      <c r="R33" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>